<commit_message>
refactor: remove unnecessary growth variables
I deleted the variables and verified that the results match the previous versions of the reordered FIM perfectly.
</commit_message>
<xml_diff>
--- a/results/07-2024/beta/contributions-07-2024.xlsx
+++ b/results/07-2024/beta/contributions-07-2024.xlsx
@@ -23996,37 +23996,37 @@
         <v>0</v>
       </c>
       <c r="D227" t="n">
-        <v>-25.4781758033178</v>
+        <v>-25.3603568154121</v>
       </c>
       <c r="E227" t="n">
-        <v>-5.40045984845628</v>
+        <v>-5.36733485897007</v>
       </c>
       <c r="F227" t="n">
-        <v>-0.991436940977191</v>
+        <v>-0.985355729530818</v>
       </c>
       <c r="G227" t="n">
-        <v>-44.023556538468</v>
+        <v>-43.7535277097379</v>
       </c>
       <c r="H227" t="n">
-        <v>7.53026154459898</v>
+        <v>7.35477245169044</v>
       </c>
       <c r="I227" t="n">
-        <v>3.93030718251723</v>
+        <v>3.83866744040209</v>
       </c>
       <c r="J227" t="n">
-        <v>0.200332369438805</v>
+        <v>0.188315746194788</v>
       </c>
       <c r="K227" t="n">
-        <v>-1.99502961502113</v>
+        <v>-1.98546310693755</v>
       </c>
       <c r="L227" t="n">
-        <v>0.0745309205516104</v>
+        <v>0.070196620832928</v>
       </c>
       <c r="M227" t="n">
-        <v>-6.4609852995825</v>
+        <v>-6.34005545484541</v>
       </c>
       <c r="N227" t="n">
-        <v>-0.650300848509651</v>
+        <v>-0.637902877025643</v>
       </c>
       <c r="O227" t="n">
         <v>0</v>
@@ -24038,52 +24038,52 @@
         <v>0</v>
       </c>
       <c r="R227" t="n">
-        <v>-0.0613377664214341</v>
+        <v>-0.0600455905134425</v>
       </c>
       <c r="S227" t="n">
-        <v>-0.0729781222825829</v>
+        <v>-0.0701375247421801</v>
       </c>
       <c r="T227" t="n">
-        <v>-0.00222443886692838</v>
+        <v>-0.00220056841775939</v>
       </c>
       <c r="U227" t="n">
-        <v>-0.00976224471265726</v>
+        <v>-0.00962750058489777</v>
       </c>
       <c r="V227" t="n">
-        <v>-0.00641616754572917</v>
+        <v>-0.00631956643125569</v>
       </c>
       <c r="W227" t="n">
-        <v>-0.00725510789376517</v>
+        <v>-0.00710093806495313</v>
       </c>
       <c r="X227" t="n">
-        <v>-0.000259576511377582</v>
+        <v>-0.000253215029984393</v>
       </c>
       <c r="Y227" t="n">
-        <v>-5.12370911398731</v>
+        <v>-5.02684404812187</v>
       </c>
       <c r="Z227" t="n">
-        <v>-0.971519413105528</v>
+        <v>-0.953307033720652</v>
       </c>
       <c r="AA227" t="n">
-        <v>-31.8700725927512</v>
+        <v>-31.713047403913</v>
       </c>
       <c r="AB227" t="n">
-        <v>-37.6316597490345</v>
+        <v>-37.400837121237</v>
       </c>
       <c r="AC227" t="n">
-        <v>9.74040240208549</v>
+        <v>9.4664891521827</v>
       </c>
       <c r="AD227" t="n">
-        <v>-13.3667480994195</v>
+        <v>-13.113794317498</v>
       </c>
       <c r="AE227" t="n">
-        <v>-3.62634569733397</v>
+        <v>-3.64730516531535</v>
       </c>
       <c r="AF227" t="n">
-        <v>-73.1280780391197</v>
+        <v>-72.7611896904654</v>
       </c>
       <c r="AG227" t="n">
-        <v>-18.624948634225</v>
+        <v>-18.5332265470615</v>
       </c>
     </row>
     <row r="228">
@@ -24109,25 +24109,25 @@
         <v>0</v>
       </c>
       <c r="H228" t="n">
-        <v>7.47914827160228</v>
+        <v>7.34102095684907</v>
       </c>
       <c r="I228" t="n">
-        <v>3.89799988312799</v>
+        <v>3.82586097335673</v>
       </c>
       <c r="J228" t="n">
-        <v>0.202965081576535</v>
+        <v>0.192008468477482</v>
       </c>
       <c r="K228" t="n">
         <v>0</v>
       </c>
       <c r="L228" t="n">
-        <v>0.0722943589185927</v>
+        <v>0.0683531961042187</v>
       </c>
       <c r="M228" t="n">
-        <v>-6.36084953430071</v>
+        <v>-6.27170976280022</v>
       </c>
       <c r="N228" t="n">
-        <v>-0.648367418331776</v>
+        <v>-0.639171165395635</v>
       </c>
       <c r="O228" t="n">
         <v>0</v>
@@ -24139,31 +24139,31 @@
         <v>0</v>
       </c>
       <c r="R228" t="n">
-        <v>-0.0514785550967738</v>
+        <v>-0.0504894757300376</v>
       </c>
       <c r="S228" t="n">
-        <v>-0.0624248395369921</v>
+        <v>-0.0599565730315564</v>
       </c>
       <c r="T228" t="n">
-        <v>-0.00282161942035962</v>
+        <v>-0.00280853422538725</v>
       </c>
       <c r="U228" t="n">
-        <v>-0.00668771367451321</v>
+        <v>-0.00660057160309517</v>
       </c>
       <c r="V228" t="n">
-        <v>-0.00575133510412946</v>
+        <v>-0.00568609239530368</v>
       </c>
       <c r="W228" t="n">
-        <v>-0.00611556126755971</v>
+        <v>-0.00599725402969195</v>
       </c>
       <c r="X228" t="n">
-        <v>-0.00025475012858761</v>
+        <v>-0.000249679355496173</v>
       </c>
       <c r="Y228" t="n">
-        <v>-5.07326162060959</v>
+        <v>-5.00161548367288</v>
       </c>
       <c r="Z228" t="n">
-        <v>-0.956813049576864</v>
+        <v>-0.943381106587583</v>
       </c>
       <c r="AA228" t="n">
         <v>0</v>
@@ -24172,19 +24172,19 @@
         <v>0</v>
       </c>
       <c r="AC228" t="n">
-        <v>11.6524075952254</v>
+        <v>11.4272435947875</v>
       </c>
       <c r="AD228" t="n">
-        <v>-13.1748259970478</v>
+        <v>-12.9876656988269</v>
       </c>
       <c r="AE228" t="n">
-        <v>-1.52241840182245</v>
+        <v>-1.56042210403939</v>
       </c>
       <c r="AF228" t="n">
-        <v>-1.52241840182245</v>
+        <v>-1.56042210403939</v>
       </c>
       <c r="AG228" t="n">
-        <v>-18.8999693112968</v>
+        <v>-18.8177481496875</v>
       </c>
     </row>
     <row r="229">
@@ -24210,25 +24210,25 @@
         <v>0</v>
       </c>
       <c r="H229" t="n">
-        <v>3.69116839388554</v>
+        <v>3.58949869709541</v>
       </c>
       <c r="I229" t="n">
-        <v>1.93251089510046</v>
+        <v>1.87937445055225</v>
       </c>
       <c r="J229" t="n">
-        <v>0.204021192136023</v>
+        <v>0.194121453611744</v>
       </c>
       <c r="K229" t="n">
         <v>0</v>
       </c>
       <c r="L229" t="n">
-        <v>0.0781911247571371</v>
+        <v>0.0746267719807314</v>
       </c>
       <c r="M229" t="n">
-        <v>-6.21416477588445</v>
+        <v>-6.15576603601462</v>
       </c>
       <c r="N229" t="n">
-        <v>-0.64639407091655</v>
+        <v>-0.640332312065784</v>
       </c>
       <c r="O229" t="n">
         <v>0</v>
@@ -24240,31 +24240,31 @@
         <v>0</v>
       </c>
       <c r="R229" t="n">
-        <v>-0.0476290650157223</v>
+        <v>-0.0468912806008519</v>
       </c>
       <c r="S229" t="n">
-        <v>-0.0574856453200442</v>
+        <v>-0.0553339920296613</v>
       </c>
       <c r="T229" t="n">
-        <v>-0.000296368724383302</v>
+        <v>-0.000296672217922851</v>
       </c>
       <c r="U229" t="n">
-        <v>-0.00304505368416158</v>
+        <v>-0.00299017072129983</v>
       </c>
       <c r="V229" t="n">
-        <v>-0.00318774760838464</v>
+        <v>-0.00315015642979454</v>
       </c>
       <c r="W229" t="n">
-        <v>-0.00569477124041224</v>
+        <v>-0.00560632495008648</v>
       </c>
       <c r="X229" t="n">
-        <v>-0.000249952018310104</v>
+        <v>-0.000246126469492257</v>
       </c>
       <c r="Y229" t="n">
-        <v>-5.03587516623575</v>
+        <v>-4.98875249625449</v>
       </c>
       <c r="Z229" t="n">
-        <v>-0.944090591852492</v>
+        <v>-0.935283001405661</v>
       </c>
       <c r="AA229" t="n">
         <v>0</v>
@@ -24273,19 +24273,19 @@
         <v>0</v>
       </c>
       <c r="AC229" t="n">
-        <v>5.90589160587917</v>
+        <v>5.73762137324014</v>
       </c>
       <c r="AD229" t="n">
-        <v>-12.9581132085007</v>
+        <v>-12.8346485691597</v>
       </c>
       <c r="AE229" t="n">
-        <v>-7.05222160262149</v>
+        <v>-7.09702719591952</v>
       </c>
       <c r="AF229" t="n">
-        <v>-7.05222160262149</v>
+        <v>-7.09702719591952</v>
       </c>
       <c r="AG229" t="n">
-        <v>-20.5303144467104</v>
+        <v>-20.4592946834256</v>
       </c>
     </row>
     <row r="230">
@@ -24311,25 +24311,25 @@
         <v>0</v>
       </c>
       <c r="H230" t="n">
-        <v>3.67898526427803</v>
+        <v>3.59482671248795</v>
       </c>
       <c r="I230" t="n">
-        <v>1.91558481981979</v>
+        <v>1.87161614428843</v>
       </c>
       <c r="J230" t="n">
-        <v>0.210642988137611</v>
+        <v>0.201719884929916</v>
       </c>
       <c r="K230" t="n">
         <v>0</v>
       </c>
       <c r="L230" t="n">
-        <v>0.0782091184917739</v>
+        <v>0.0750185918376533</v>
       </c>
       <c r="M230" t="n">
-        <v>-6.2233653994001</v>
+        <v>-6.19421666045563</v>
       </c>
       <c r="N230" t="n">
-        <v>-0.644613922219932</v>
+        <v>-0.641594706452758</v>
       </c>
       <c r="O230" t="n">
         <v>0</v>
@@ -24341,31 +24341,31 @@
         <v>0</v>
       </c>
       <c r="R230" t="n">
-        <v>-0.04388804081668</v>
+        <v>-0.0433750387633546</v>
       </c>
       <c r="S230" t="n">
-        <v>-0.0519625805553657</v>
+        <v>-0.0500848040394384</v>
       </c>
       <c r="T230" t="n">
-        <v>-0.000290772093670924</v>
+        <v>-0.000292464280444016</v>
       </c>
       <c r="U230" t="n">
-        <v>-0.00135627825793918</v>
+        <v>-0.00131578199585016</v>
       </c>
       <c r="V230" t="n">
-        <v>-0.00180042581795246</v>
+        <v>-0.00177785492761094</v>
       </c>
       <c r="W230" t="n">
-        <v>-0.00525729602798994</v>
+        <v>-0.00519572632675305</v>
       </c>
       <c r="X230" t="n">
-        <v>-0.00024529579453769</v>
+        <v>-0.000242649783946854</v>
       </c>
       <c r="Y230" t="n">
-        <v>-5.00010415140023</v>
+        <v>-4.97668487240074</v>
       </c>
       <c r="Z230" t="n">
-        <v>-0.931708895404838</v>
+        <v>-0.927344996192522</v>
       </c>
       <c r="AA230" t="n">
         <v>0</v>
@@ -24374,19 +24374,19 @@
         <v>0</v>
       </c>
       <c r="AC230" t="n">
-        <v>5.8834221907272</v>
+        <v>5.74318133354395</v>
       </c>
       <c r="AD230" t="n">
-        <v>-12.9045930577892</v>
+        <v>-12.8421255556191</v>
       </c>
       <c r="AE230" t="n">
-        <v>-7.02117086706204</v>
+        <v>-7.0989442220751</v>
       </c>
       <c r="AF230" t="n">
-        <v>-7.02117086706204</v>
+        <v>-7.0989442220751</v>
       </c>
       <c r="AG230" t="n">
-        <v>-22.1809722276564</v>
+        <v>-22.1293958031249</v>
       </c>
     </row>
     <row r="231">
@@ -24412,19 +24412,19 @@
         <v>0</v>
       </c>
       <c r="H231" t="n">
-        <v>3.63497630906841</v>
+        <v>3.56797560038849</v>
       </c>
       <c r="I231" t="n">
-        <v>1.89870463611531</v>
+        <v>1.86366959291199</v>
       </c>
       <c r="J231" t="n">
-        <v>0.211458115264035</v>
+        <v>0.203512880998237</v>
       </c>
       <c r="K231" t="n">
         <v>0</v>
       </c>
       <c r="L231" t="n">
-        <v>0.0783185251358729</v>
+        <v>0.0754912038313918</v>
       </c>
       <c r="M231" t="n">
         <v>0</v>
@@ -24442,25 +24442,25 @@
         <v>0</v>
       </c>
       <c r="R231" t="n">
-        <v>-0.0261020994028258</v>
+        <v>-0.0257943200696954</v>
       </c>
       <c r="S231" t="n">
-        <v>-0.0442518267126678</v>
+        <v>-0.0426156321678845</v>
       </c>
       <c r="T231" t="n">
-        <v>-0.000285357584419229</v>
+        <v>-0.000288415037551126</v>
       </c>
       <c r="U231" t="n">
-        <v>-0.00102721741261374</v>
+        <v>-0.000993036064356082</v>
       </c>
       <c r="V231" t="n">
-        <v>-0.00152065689196695</v>
+        <v>-0.00150650320584166</v>
       </c>
       <c r="W231" t="n">
-        <v>-0.00312501588885578</v>
+        <v>-0.00308802944272969</v>
       </c>
       <c r="X231" t="n">
-        <v>-0.0000823369980046373</v>
+        <v>-0.0000808382464693936</v>
       </c>
       <c r="Y231" t="n">
         <v>0</v>
@@ -24475,19 +24475,19 @@
         <v>0</v>
       </c>
       <c r="AC231" t="n">
-        <v>5.82345758558363</v>
+        <v>5.71064927813011</v>
       </c>
       <c r="AD231" t="n">
-        <v>-0.0763945108913539</v>
+        <v>-0.0743667742345278</v>
       </c>
       <c r="AE231" t="n">
-        <v>5.74706307469227</v>
+        <v>5.63628250389558</v>
       </c>
       <c r="AF231" t="n">
-        <v>5.74706307469227</v>
+        <v>5.63628250389558</v>
       </c>
       <c r="AG231" t="n">
-        <v>-2.46218694920342</v>
+        <v>-2.53002775453461</v>
       </c>
     </row>
     <row r="232">
@@ -24513,19 +24513,19 @@
         <v>0</v>
       </c>
       <c r="H232" t="n">
-        <v>3.59270603794707</v>
+        <v>3.54271794870323</v>
       </c>
       <c r="I232" t="n">
-        <v>1.88175430149973</v>
+        <v>1.85560567102224</v>
       </c>
       <c r="J232" t="n">
-        <v>0.212404202286098</v>
+        <v>0.205447474209381</v>
       </c>
       <c r="K232" t="n">
         <v>0</v>
       </c>
       <c r="L232" t="n">
-        <v>0.0780272491649796</v>
+        <v>0.0755660779655674</v>
       </c>
       <c r="M232" t="n">
         <v>0</v>
@@ -24543,25 +24543,25 @@
         <v>0</v>
       </c>
       <c r="R232" t="n">
-        <v>-0.0144077486405538</v>
+        <v>-0.0142221840007382</v>
       </c>
       <c r="S232" t="n">
-        <v>-0.0438971540573117</v>
+        <v>-0.0424678318154382</v>
       </c>
       <c r="T232" t="n">
-        <v>-0.000280082191413928</v>
+        <v>-0.000284477599182361</v>
       </c>
       <c r="U232" t="n">
-        <v>-0.00101258848718434</v>
+        <v>-0.000983210364684009</v>
       </c>
       <c r="V232" t="n">
-        <v>-0.0012582682069139</v>
+        <v>-0.00125123560161194</v>
       </c>
       <c r="W232" t="n">
-        <v>-0.00172780972816472</v>
+        <v>-0.00170545512477903</v>
       </c>
       <c r="X232" t="n">
-        <v>-0.0000808377625138823</v>
+        <v>-0.0000797243746749887</v>
       </c>
       <c r="Y232" t="n">
         <v>0</v>
@@ -24576,19 +24576,19 @@
         <v>0</v>
       </c>
       <c r="AC232" t="n">
-        <v>5.76489179089788</v>
+        <v>5.67933717190042</v>
       </c>
       <c r="AD232" t="n">
-        <v>-0.0626644890740563</v>
+        <v>-0.0609941188811087</v>
       </c>
       <c r="AE232" t="n">
-        <v>5.70222730182382</v>
+        <v>5.61834305301932</v>
       </c>
       <c r="AF232" t="n">
-        <v>5.70222730182382</v>
+        <v>5.61834305301932</v>
       </c>
       <c r="AG232" t="n">
-        <v>-0.656025523291855</v>
+        <v>-0.735336465269932</v>
       </c>
     </row>
     <row r="233">
@@ -24614,19 +24614,19 @@
         <v>0</v>
       </c>
       <c r="H233" t="n">
-        <v>3.55127046865678</v>
+        <v>3.51798426581115</v>
       </c>
       <c r="I233" t="n">
-        <v>1.86477390521435</v>
+        <v>1.84737334931225</v>
       </c>
       <c r="J233" t="n">
-        <v>0.212540978085828</v>
+        <v>0.206557993611421</v>
       </c>
       <c r="K233" t="n">
         <v>0</v>
       </c>
       <c r="L233" t="n">
-        <v>0.0771733197159231</v>
+        <v>0.0750701787467338</v>
       </c>
       <c r="M233" t="n">
         <v>0</v>
@@ -24644,25 +24644,25 @@
         <v>0</v>
       </c>
       <c r="R233" t="n">
-        <v>-0.0141455741364896</v>
+        <v>-0.0140270396725678</v>
       </c>
       <c r="S233" t="n">
-        <v>-0.0447903056036093</v>
+        <v>-0.0435622537872699</v>
       </c>
       <c r="T233" t="n">
-        <v>0.000201101794547248</v>
+        <v>0.000195375965316679</v>
       </c>
       <c r="U233" t="n">
-        <v>-0.00100762032322826</v>
+        <v>-0.000982897253508742</v>
       </c>
       <c r="V233" t="n">
-        <v>-0.000244548204408272</v>
+        <v>-0.000243400907868585</v>
       </c>
       <c r="W233" t="n">
-        <v>-0.00170849615728338</v>
+        <v>-0.00169417961741289</v>
       </c>
       <c r="X233" t="n">
-        <v>-0.0000793678239583342</v>
+        <v>-0.0000786302761828208</v>
       </c>
       <c r="Y233" t="n">
         <v>0</v>
@@ -24677,19 +24677,19 @@
         <v>0</v>
       </c>
       <c r="AC233" t="n">
-        <v>5.70575867167288</v>
+        <v>5.64698578748156</v>
       </c>
       <c r="AD233" t="n">
-        <v>-0.0617748104544299</v>
+        <v>-0.0603930255494941</v>
       </c>
       <c r="AE233" t="n">
-        <v>5.64398386121845</v>
+        <v>5.58659276193206</v>
       </c>
       <c r="AF233" t="n">
-        <v>5.64398386121845</v>
+        <v>5.58659276193206</v>
       </c>
       <c r="AG233" t="n">
-        <v>2.51802584266813</v>
+        <v>2.43556852419296</v>
       </c>
     </row>
     <row r="234">
@@ -24715,19 +24715,19 @@
         <v>0</v>
       </c>
       <c r="H234" t="n">
-        <v>3.54722251898612</v>
+        <v>3.53049854837285</v>
       </c>
       <c r="I234" t="n">
-        <v>1.84599635786205</v>
+        <v>1.83729310096856</v>
       </c>
       <c r="J234" t="n">
-        <v>0.212698222991494</v>
+        <v>0.207682823870142</v>
       </c>
       <c r="K234" t="n">
         <v>0</v>
       </c>
       <c r="L234" t="n">
-        <v>0.0764437491025072</v>
+        <v>0.0746923475182203</v>
       </c>
       <c r="M234" t="n">
         <v>0</v>
@@ -24745,25 +24745,25 @@
         <v>0</v>
       </c>
       <c r="R234" t="n">
-        <v>-0.0111311756526391</v>
+        <v>-0.0110786958734571</v>
       </c>
       <c r="S234" t="n">
-        <v>-0.0435795230456598</v>
+        <v>-0.0425555718373158</v>
       </c>
       <c r="T234" t="n">
-        <v>0.000197481144560533</v>
+        <v>0.000192670439824647</v>
       </c>
       <c r="U234" t="n">
-        <v>-0.00101257451916756</v>
+        <v>-0.000992460186024399</v>
       </c>
       <c r="V234" t="n">
         <v>0</v>
       </c>
       <c r="W234" t="n">
-        <v>-0.00134441844813657</v>
+        <v>-0.00133807996373131</v>
       </c>
       <c r="X234" t="n">
-        <v>-0.0000779182295684739</v>
+        <v>-0.0000775508711141996</v>
       </c>
       <c r="Y234" t="n">
         <v>0</v>
@@ -24778,19 +24778,19 @@
         <v>0</v>
       </c>
       <c r="AC234" t="n">
-        <v>5.68236084894217</v>
+        <v>5.65016682072977</v>
       </c>
       <c r="AD234" t="n">
-        <v>-0.056948128750611</v>
+        <v>-0.0558496882918182</v>
       </c>
       <c r="AE234" t="n">
-        <v>5.62541272019156</v>
+        <v>5.59431713243795</v>
       </c>
       <c r="AF234" t="n">
-        <v>5.62541272019156</v>
+        <v>5.59431713243795</v>
       </c>
       <c r="AG234" t="n">
-        <v>5.67967173948153</v>
+        <v>5.60888386282123</v>
       </c>
     </row>
     <row r="235">
@@ -24822,13 +24822,13 @@
         <v>0</v>
       </c>
       <c r="J235" t="n">
-        <v>0.212942315570546</v>
+        <v>0.208901120628369</v>
       </c>
       <c r="K235" t="n">
         <v>0</v>
       </c>
       <c r="L235" t="n">
-        <v>0.0757348270278107</v>
+        <v>0.0743339188759051</v>
       </c>
       <c r="M235" t="n">
         <v>0</v>
@@ -24849,13 +24849,13 @@
         <v>0</v>
       </c>
       <c r="S235" t="n">
-        <v>-0.0328921109306041</v>
+        <v>-0.0320677894322871</v>
       </c>
       <c r="T235" t="n">
-        <v>0.000193971364641815</v>
+        <v>0.000190064068152045</v>
       </c>
       <c r="U235" t="n">
-        <v>-0.000597858145735165</v>
+        <v>-0.000582408435796675</v>
       </c>
       <c r="V235" t="n">
         <v>0</v>
@@ -24879,19 +24879,19 @@
         <v>0</v>
       </c>
       <c r="AC235" t="n">
-        <v>0.288677142598356</v>
+        <v>0.283235039504274</v>
       </c>
       <c r="AD235" t="n">
-        <v>-0.0332959977116974</v>
+        <v>-0.0324601337999317</v>
       </c>
       <c r="AE235" t="n">
-        <v>0.255381144886659</v>
+        <v>0.250774905704343</v>
       </c>
       <c r="AF235" t="n">
-        <v>0.255381144886659</v>
+        <v>0.250774905704343</v>
       </c>
       <c r="AG235" t="n">
-        <v>4.30675125703013</v>
+        <v>4.26250696327342</v>
       </c>
     </row>
     <row r="236">
@@ -24923,13 +24923,13 @@
         <v>0</v>
       </c>
       <c r="J236" t="n">
-        <v>0.213133883917379</v>
+        <v>0.210090249656128</v>
       </c>
       <c r="K236" t="n">
         <v>0</v>
       </c>
       <c r="L236" t="n">
-        <v>0.0747650089411367</v>
+        <v>0.0737190428986672</v>
       </c>
       <c r="M236" t="n">
         <v>0</v>
@@ -24950,13 +24950,13 @@
         <v>0</v>
       </c>
       <c r="S236" t="n">
-        <v>-0.0325131794793199</v>
+        <v>-0.0318421166831904</v>
       </c>
       <c r="T236" t="n">
-        <v>0.000190439834478947</v>
+        <v>0.00018744028906882</v>
       </c>
       <c r="U236" t="n">
-        <v>-0.000596128215914088</v>
+        <v>-0.000583462254165791</v>
       </c>
       <c r="V236" t="n">
         <v>0</v>
@@ -24980,19 +24980,19 @@
         <v>0</v>
       </c>
       <c r="AC236" t="n">
-        <v>0.287898892858515</v>
+        <v>0.283809292554795</v>
       </c>
       <c r="AD236" t="n">
-        <v>-0.0329188678607551</v>
+        <v>-0.0322381386482874</v>
       </c>
       <c r="AE236" t="n">
-        <v>0.25498002499776</v>
+        <v>0.251571153906508</v>
       </c>
       <c r="AF236" t="n">
-        <v>0.25498002499776</v>
+        <v>0.251571153906508</v>
       </c>
       <c r="AG236" t="n">
-        <v>2.94493943782361</v>
+        <v>2.92081398849522</v>
       </c>
     </row>
     <row r="237">
@@ -25024,13 +25024,13 @@
         <v>0</v>
       </c>
       <c r="J237" t="n">
-        <v>0.21332052110136</v>
+        <v>0.211284270734589</v>
       </c>
       <c r="K237" t="n">
         <v>0</v>
       </c>
       <c r="L237" t="n">
-        <v>0.0734208633555086</v>
+        <v>0.0727283511369669</v>
       </c>
       <c r="M237" t="n">
         <v>0</v>
@@ -25051,13 +25051,13 @@
         <v>0</v>
       </c>
       <c r="S237" t="n">
-        <v>-0.0338254618496985</v>
+        <v>-0.0333073621121984</v>
       </c>
       <c r="T237" t="n">
-        <v>0.000440132631366132</v>
+        <v>0.000438032242245689</v>
       </c>
       <c r="U237" t="n">
-        <v>-0.000596662815721709</v>
+        <v>-0.000586800181445484</v>
       </c>
       <c r="V237" t="n">
         <v>0</v>
@@ -25081,19 +25081,19 @@
         <v>0</v>
       </c>
       <c r="AC237" t="n">
-        <v>0.286741384456868</v>
+        <v>0.284012621871556</v>
       </c>
       <c r="AD237" t="n">
-        <v>-0.0339819920340541</v>
+        <v>-0.0334561300513982</v>
       </c>
       <c r="AE237" t="n">
-        <v>0.252759392422814</v>
+        <v>0.250556491820158</v>
       </c>
       <c r="AF237" t="n">
-        <v>0.252759392422814</v>
+        <v>0.250556491820158</v>
       </c>
       <c r="AG237" t="n">
-        <v>1.5971333206247</v>
+        <v>1.58680492096724</v>
       </c>
     </row>
     <row r="238">
@@ -25125,13 +25125,13 @@
         <v>0</v>
       </c>
       <c r="J238" t="n">
-        <v>0.21350434096293</v>
+        <v>0.21248178173747</v>
       </c>
       <c r="K238" t="n">
         <v>0</v>
       </c>
       <c r="L238" t="n">
-        <v>0.0717382658642193</v>
+        <v>0.0713946820979732</v>
       </c>
       <c r="M238" t="n">
         <v>0</v>
@@ -25152,13 +25152,13 @@
         <v>0</v>
       </c>
       <c r="S238" t="n">
-        <v>-0.0329535507630979</v>
+        <v>-0.0325953617878963</v>
       </c>
       <c r="T238" t="n">
         <v>0</v>
       </c>
       <c r="U238" t="n">
-        <v>-0.000498229107606513</v>
+        <v>-0.000491184148601089</v>
       </c>
       <c r="V238" t="n">
         <v>0</v>
@@ -25182,19 +25182,19 @@
         <v>0</v>
       </c>
       <c r="AC238" t="n">
-        <v>0.285242606827149</v>
+        <v>0.283876463835443</v>
       </c>
       <c r="AD238" t="n">
-        <v>-0.0334517798707044</v>
+        <v>-0.0330865459364974</v>
       </c>
       <c r="AE238" t="n">
-        <v>0.251790826956445</v>
+        <v>0.250789917898946</v>
       </c>
       <c r="AF238" t="n">
-        <v>0.251790826956445</v>
+        <v>0.250789917898946</v>
       </c>
       <c r="AG238" t="n">
-        <v>0.253727847315923</v>
+        <v>0.25092311733249</v>
       </c>
     </row>
     <row r="239">
@@ -25253,13 +25253,13 @@
         <v>0</v>
       </c>
       <c r="S239" t="n">
-        <v>-0.0104390726378308</v>
+        <v>-0.0102384425769539</v>
       </c>
       <c r="T239" t="n">
         <v>0</v>
       </c>
       <c r="U239" t="n">
-        <v>-0.000393528371012856</v>
+        <v>-0.00038886337800323</v>
       </c>
       <c r="V239" t="n">
         <v>0</v>
@@ -25286,16 +25286,16 @@
         <v>0</v>
       </c>
       <c r="AD239" t="n">
-        <v>-0.0108326010088437</v>
+        <v>-0.0106273059549571</v>
       </c>
       <c r="AE239" t="n">
-        <v>-0.0108326010088437</v>
+        <v>-0.0106273059549571</v>
       </c>
       <c r="AF239" t="n">
-        <v>-0.0108326010088437</v>
+        <v>-0.0106273059549571</v>
       </c>
       <c r="AG239" t="n">
-        <v>0.187174410842048</v>
+        <v>0.185572564417665</v>
       </c>
     </row>
     <row r="240">
@@ -25354,13 +25354,13 @@
         <v>0</v>
       </c>
       <c r="S240" t="n">
-        <v>-0.010348254093353</v>
+        <v>-0.0101974863743186</v>
       </c>
       <c r="T240" t="n">
         <v>0</v>
       </c>
       <c r="U240" t="n">
-        <v>-0.00029159818734561</v>
+        <v>-0.000288816249438213</v>
       </c>
       <c r="V240" t="n">
         <v>0</v>
@@ -25387,16 +25387,16 @@
         <v>0</v>
       </c>
       <c r="AD240" t="n">
-        <v>-0.0106398522806986</v>
+        <v>-0.0104863026237568</v>
       </c>
       <c r="AE240" t="n">
-        <v>-0.0106398522806986</v>
+        <v>-0.0104863026237568</v>
       </c>
       <c r="AF240" t="n">
-        <v>-0.0106398522806986</v>
+        <v>-0.0104863026237568</v>
       </c>
       <c r="AG240" t="n">
-        <v>0.120769441522433</v>
+        <v>0.120058200285099</v>
       </c>
     </row>
     <row r="241">
@@ -25455,13 +25455,13 @@
         <v>0</v>
       </c>
       <c r="S241" t="n">
-        <v>-0.0107062066615528</v>
+        <v>-0.0106048896560545</v>
       </c>
       <c r="T241" t="n">
         <v>0</v>
       </c>
       <c r="U241" t="n">
-        <v>-0.000192450503772596</v>
+        <v>-0.000191064728518691</v>
       </c>
       <c r="V241" t="n">
         <v>0</v>
@@ -25488,16 +25488,16 @@
         <v>0</v>
       </c>
       <c r="AD241" t="n">
-        <v>-0.0108986571653254</v>
+        <v>-0.0107959543845732</v>
       </c>
       <c r="AE241" t="n">
-        <v>-0.0108986571653254</v>
+        <v>-0.0107959543845732</v>
       </c>
       <c r="AF241" t="n">
-        <v>-0.0108986571653254</v>
+        <v>-0.0107959543845732</v>
       </c>
       <c r="AG241" t="n">
-        <v>0.0548549291253979</v>
+        <v>0.0547200887339165</v>
       </c>
     </row>
     <row r="242">
@@ -25556,13 +25556,13 @@
         <v>0</v>
       </c>
       <c r="S242" t="n">
-        <v>-0.0103867386457179</v>
+        <v>-0.0103368301256772</v>
       </c>
       <c r="T242" t="n">
         <v>0</v>
       </c>
       <c r="U242" t="n">
-        <v>-0.0000960384429382324</v>
+        <v>-0.0000955769759929711</v>
       </c>
       <c r="V242" t="n">
         <v>0</v>
@@ -25589,16 +25589,16 @@
         <v>0</v>
       </c>
       <c r="AD242" t="n">
-        <v>-0.0104827770886562</v>
+        <v>-0.0104324071016701</v>
       </c>
       <c r="AE242" t="n">
-        <v>-0.0104827770886562</v>
+        <v>-0.0104324071016701</v>
       </c>
       <c r="AF242" t="n">
-        <v>-0.0104827770886562</v>
+        <v>-0.0104324071016701</v>
       </c>
       <c r="AG242" t="n">
-        <v>-0.0107134718858773</v>
+        <v>-0.0105854925162375</v>
       </c>
     </row>
     <row r="243">
@@ -25699,7 +25699,7 @@
         <v>0</v>
       </c>
       <c r="AG243" t="n">
-        <v>-0.00800532163366641</v>
+        <v>-0.00792866602749823</v>
       </c>
     </row>
     <row r="244">
@@ -25800,7 +25800,7 @@
         <v>0</v>
       </c>
       <c r="AG244" t="n">
-        <v>-0.00534535856349176</v>
+        <v>-0.00530709037155903</v>
       </c>
     </row>
     <row r="245">
@@ -25901,7 +25901,7 @@
         <v>0</v>
       </c>
       <c r="AG245" t="n">
-        <v>-0.0026206942721604</v>
+        <v>-0.00260810177541573</v>
       </c>
     </row>
     <row r="246">
@@ -26002,7 +26002,7 @@
         <v>0</v>
       </c>
       <c r="AG246" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="247">
@@ -26103,7 +26103,7 @@
         <v>0</v>
       </c>
       <c r="AG247" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="248">
@@ -26204,7 +26204,7 @@
         <v>0</v>
       </c>
       <c r="AG248" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="249">
@@ -26305,7 +26305,7 @@
         <v>0</v>
       </c>
       <c r="AG249" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="250">
@@ -26406,7 +26406,7 @@
         <v>0</v>
       </c>
       <c r="AG250" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="251">
@@ -26507,7 +26507,7 @@
         <v>0</v>
       </c>
       <c r="AG251" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="252">
@@ -26608,7 +26608,7 @@
         <v>0</v>
       </c>
       <c r="AG252" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="253">
@@ -26709,7 +26709,7 @@
         <v>0</v>
       </c>
       <c r="AG253" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="254">
@@ -26810,7 +26810,7 @@
         <v>0</v>
       </c>
       <c r="AG254" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="255">
@@ -26911,7 +26911,7 @@
         <v>0</v>
       </c>
       <c r="AG255" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="256">
@@ -27012,7 +27012,7 @@
         <v>0</v>
       </c>
       <c r="AG256" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="257">
@@ -27113,7 +27113,7 @@
         <v>0</v>
       </c>
       <c r="AG257" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="258">
@@ -27214,7 +27214,7 @@
         <v>0</v>
       </c>
       <c r="AG258" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="259">
@@ -27315,7 +27315,7 @@
         <v>0</v>
       </c>
       <c r="AG259" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
     <row r="260">
@@ -27416,7 +27416,7 @@
         <v>0</v>
       </c>
       <c r="AG260" t="n">
-        <v>0.00000000000000364422034215828</v>
+        <v>0.00000000000000180151032980191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: improve clarity of input data pipeline
Many changes were made, primarily through explicitly naming input variables and their subsequent transformations.
</commit_message>
<xml_diff>
--- a/results/07-2024/beta/contributions-07-2024.xlsx
+++ b/results/07-2024/beta/contributions-07-2024.xlsx
@@ -23251,7 +23251,7 @@
         <v>-0.00257510812555391</v>
       </c>
       <c r="Y219" t="n">
-        <v>-0.120931885598694</v>
+        <v>-3.24271824541152</v>
       </c>
       <c r="Z219" t="n">
         <v>0.0915937580995</v>
@@ -23266,16 +23266,16 @@
         <v>0.203639383205674</v>
       </c>
       <c r="AD219" t="n">
-        <v>-0.518073574342654</v>
+        <v>-3.63985993415548</v>
       </c>
       <c r="AE219" t="n">
-        <v>-0.31443419113698</v>
+        <v>-3.4362205509498</v>
       </c>
       <c r="AF219" t="n">
-        <v>-0.792147721191593</v>
+        <v>-3.91393408100442</v>
       </c>
       <c r="AG219" t="n">
-        <v>-0.0793489214949135</v>
+        <v>-0.859795511448119</v>
       </c>
     </row>
     <row r="220">
@@ -23352,7 +23352,7 @@
         <v>-0.000460358230979371</v>
       </c>
       <c r="Y220" t="n">
-        <v>0.088397837426483</v>
+        <v>-3.00857089304738</v>
       </c>
       <c r="Z220" t="n">
         <v>0.0402455803781892</v>
@@ -23367,16 +23367,16 @@
         <v>0.273124597025881</v>
       </c>
       <c r="AD220" t="n">
-        <v>-0.283301574583727</v>
+        <v>-3.38027030505759</v>
       </c>
       <c r="AE220" t="n">
-        <v>-0.0101769775578465</v>
+        <v>-3.10714570803171</v>
       </c>
       <c r="AF220" t="n">
-        <v>-0.416907272604143</v>
+        <v>-3.51387600307801</v>
       </c>
       <c r="AG220" t="n">
-        <v>-0.288164791241573</v>
+        <v>-1.84285356381324</v>
       </c>
     </row>
     <row r="221">
@@ -23408,7 +23408,7 @@
         <v>0.0639536473026019</v>
       </c>
       <c r="J221" t="n">
-        <v>-0.0609488861054173</v>
+        <v>-0.0609488861054172</v>
       </c>
       <c r="K221" t="n">
         <v>0.0314974458604034</v>
@@ -23420,7 +23420,7 @@
         <v>0.0953813358267898</v>
       </c>
       <c r="N221" t="n">
-        <v>0.0665666792477965</v>
+        <v>0.0665666792477964</v>
       </c>
       <c r="O221" t="n">
         <v>0</v>
@@ -23438,7 +23438,7 @@
         <v>-0.101088950824126</v>
       </c>
       <c r="T221" t="n">
-        <v>-0.0280405483059011</v>
+        <v>-0.028040548305901</v>
       </c>
       <c r="U221" t="n">
         <v>-0.0214805665186662</v>
@@ -23453,7 +23453,7 @@
         <v>-0.000427312939056426</v>
       </c>
       <c r="Y221" t="n">
-        <v>0.0428884779630856</v>
+        <v>-3.02947656186133</v>
       </c>
       <c r="Z221" t="n">
         <v>0.163361542193921</v>
@@ -23468,16 +23468,16 @@
         <v>0.233504338998095</v>
       </c>
       <c r="AD221" t="n">
-        <v>0.0628664281438527</v>
+        <v>-3.00949861168056</v>
       </c>
       <c r="AE221" t="n">
-        <v>0.296370767141948</v>
+        <v>-2.77599427268247</v>
       </c>
       <c r="AF221" t="n">
-        <v>0.168918177547001</v>
+        <v>-2.90344686227742</v>
       </c>
       <c r="AG221" t="n">
-        <v>-0.284301312961626</v>
+        <v>-2.6070813454894</v>
       </c>
     </row>
     <row r="222">
@@ -23554,7 +23554,7 @@
         <v>-0.000633207294966489</v>
       </c>
       <c r="Y222" t="n">
-        <v>0.0463959848314359</v>
+        <v>-2.9995609315951</v>
       </c>
       <c r="Z222" t="n">
         <v>0.00166196924893043</v>
@@ -23569,16 +23569,16 @@
         <v>-0.060565971679117</v>
       </c>
       <c r="AD222" t="n">
-        <v>-0.190109689906182</v>
+        <v>-3.23606660633272</v>
       </c>
       <c r="AE222" t="n">
-        <v>-0.250675661585299</v>
+        <v>-3.29663257801184</v>
       </c>
       <c r="AF222" t="n">
-        <v>-0.369115608889997</v>
+        <v>-3.41507252531653</v>
       </c>
       <c r="AG222" t="n">
-        <v>-0.352313106284686</v>
+        <v>-3.4365823679191</v>
       </c>
     </row>
     <row r="223">
@@ -23655,7 +23655,7 @@
         <v>-0.00132113680474515</v>
       </c>
       <c r="Y223" t="n">
-        <v>-0.0149421958634524</v>
+        <v>-0.0491246038173944</v>
       </c>
       <c r="Z223" t="n">
         <v>-0.0242858019237184</v>
@@ -23670,16 +23670,16 @@
         <v>-0.139258186554956</v>
       </c>
       <c r="AD223" t="n">
-        <v>-0.359859513326051</v>
+        <v>-0.394041921279993</v>
       </c>
       <c r="AE223" t="n">
-        <v>-0.499117699881007</v>
+        <v>-0.533300107834949</v>
       </c>
       <c r="AF223" t="n">
-        <v>-0.604018090056283</v>
+        <v>-0.638200498010225</v>
       </c>
       <c r="AG223" t="n">
-        <v>-0.305280698500859</v>
+        <v>-2.61764897217055</v>
       </c>
     </row>
     <row r="224">
@@ -23729,7 +23729,7 @@
         <v>0</v>
       </c>
       <c r="P224" t="n">
-        <v>-0.000981412659284884</v>
+        <v>-0.000981412659284883</v>
       </c>
       <c r="Q224" t="n">
         <v>0</v>
@@ -23747,7 +23747,7 @@
         <v>-0.0134766162106087</v>
       </c>
       <c r="V224" t="n">
-        <v>-0.00833393661051035</v>
+        <v>-0.00833393661051034</v>
       </c>
       <c r="W224" t="n">
         <v>0.000199372282329125</v>
@@ -23756,7 +23756,7 @@
         <v>-0.000340721025477894</v>
       </c>
       <c r="Y224" t="n">
-        <v>-0.0259224157996425</v>
+        <v>-0.0527523123288485</v>
       </c>
       <c r="Z224" t="n">
         <v>-0.0260792374631428</v>
@@ -23771,16 +23771,16 @@
         <v>-0.082606882215624</v>
       </c>
       <c r="AD224" t="n">
-        <v>-0.226238838922083</v>
+        <v>-0.253068735451289</v>
       </c>
       <c r="AE224" t="n">
-        <v>-0.308845721137707</v>
+        <v>-0.335675617666913</v>
       </c>
       <c r="AF224" t="n">
-        <v>-0.422335693535425</v>
+        <v>-0.449165590064631</v>
       </c>
       <c r="AG224" t="n">
-        <v>-0.306637803733679</v>
+        <v>-1.8514713689172</v>
       </c>
     </row>
     <row r="225">
@@ -23836,7 +23836,7 @@
         <v>0</v>
       </c>
       <c r="R225" t="n">
-        <v>-0.002946489937161</v>
+        <v>-0.00294648993716099</v>
       </c>
       <c r="S225" t="n">
         <v>-0.0302453020434886</v>
@@ -23857,7 +23857,7 @@
         <v>-0.000333770556234235</v>
       </c>
       <c r="Y225" t="n">
-        <v>-0.00919212637130683</v>
+        <v>-0.0473109382502551</v>
       </c>
       <c r="Z225" t="n">
         <v>-0.0233891774362589</v>
@@ -23869,19 +23869,19 @@
         <v>-0.0517915188428103</v>
       </c>
       <c r="AC225" t="n">
-        <v>-0.0876249557515836</v>
+        <v>-0.0876249557515835</v>
       </c>
       <c r="AD225" t="n">
-        <v>-0.197470921923654</v>
+        <v>-0.235589733802603</v>
       </c>
       <c r="AE225" t="n">
-        <v>-0.285095877675238</v>
+        <v>-0.323214689554186</v>
       </c>
       <c r="AF225" t="n">
-        <v>-0.530841060967046</v>
+        <v>-0.568959872845994</v>
       </c>
       <c r="AG225" t="n">
-        <v>-0.481577613362191</v>
+        <v>-1.26784962155935</v>
       </c>
     </row>
     <row r="226">
@@ -23958,7 +23958,7 @@
         <v>-0.000327241566119516</v>
       </c>
       <c r="Y226" t="n">
-        <v>0.00699042861733471</v>
+        <v>-0.0421640022999755</v>
       </c>
       <c r="Z226" t="n">
         <v>-0.0208446792156265</v>
@@ -23973,16 +23973,16 @@
         <v>-0.0515940386867133</v>
       </c>
       <c r="AD226" t="n">
-        <v>-0.150819031648804</v>
+        <v>-0.199973462566114</v>
       </c>
       <c r="AE226" t="n">
-        <v>-0.202413070335517</v>
+        <v>-0.251567501252828</v>
       </c>
       <c r="AF226" t="n">
-        <v>-0.418539743277965</v>
+        <v>-0.467694174195275</v>
       </c>
       <c r="AG226" t="n">
-        <v>-0.493933646959183</v>
+        <v>-0.531005033779035</v>
       </c>
     </row>
     <row r="227">
@@ -23996,37 +23996,37 @@
         <v>0</v>
       </c>
       <c r="D227" t="n">
-        <v>-25.3603568154121</v>
+        <v>-25.4781758033177</v>
       </c>
       <c r="E227" t="n">
-        <v>-5.36733485897007</v>
+        <v>-5.40045984845628</v>
       </c>
       <c r="F227" t="n">
-        <v>-0.985355729530818</v>
+        <v>-0.991436940977191</v>
       </c>
       <c r="G227" t="n">
-        <v>-43.7535277097379</v>
+        <v>-44.023556538468</v>
       </c>
       <c r="H227" t="n">
-        <v>7.35477245169044</v>
+        <v>7.53026154459898</v>
       </c>
       <c r="I227" t="n">
-        <v>3.83866744040209</v>
+        <v>3.93030718251723</v>
       </c>
       <c r="J227" t="n">
-        <v>0.188315746194788</v>
+        <v>0.200332369438805</v>
       </c>
       <c r="K227" t="n">
-        <v>-1.98546310693755</v>
+        <v>-1.99502961502113</v>
       </c>
       <c r="L227" t="n">
-        <v>0.070196620832928</v>
+        <v>0.0745309205516103</v>
       </c>
       <c r="M227" t="n">
-        <v>-6.34005545484541</v>
+        <v>-6.4609852995825</v>
       </c>
       <c r="N227" t="n">
-        <v>-0.637902877025643</v>
+        <v>-0.650300848509651</v>
       </c>
       <c r="O227" t="n">
         <v>0</v>
@@ -24038,52 +24038,52 @@
         <v>0</v>
       </c>
       <c r="R227" t="n">
-        <v>-0.0600455905134425</v>
+        <v>-0.0613377664214341</v>
       </c>
       <c r="S227" t="n">
-        <v>-0.0701375247421801</v>
+        <v>-0.0729781222825829</v>
       </c>
       <c r="T227" t="n">
-        <v>-0.00220056841775939</v>
+        <v>-0.00222443886692838</v>
       </c>
       <c r="U227" t="n">
-        <v>-0.00962750058489777</v>
+        <v>-0.00976224471265726</v>
       </c>
       <c r="V227" t="n">
-        <v>-0.00631956643125569</v>
+        <v>-0.00641616754572917</v>
       </c>
       <c r="W227" t="n">
-        <v>-0.00710093806495313</v>
+        <v>-0.00725510789376517</v>
       </c>
       <c r="X227" t="n">
-        <v>-0.000253215029984393</v>
+        <v>-0.000259576511377582</v>
       </c>
       <c r="Y227" t="n">
-        <v>-5.02684404812187</v>
+        <v>-1.96516081369773</v>
       </c>
       <c r="Z227" t="n">
-        <v>-0.953307033720652</v>
+        <v>-0.971519413105528</v>
       </c>
       <c r="AA227" t="n">
-        <v>-31.713047403913</v>
+        <v>-31.8700725927512</v>
       </c>
       <c r="AB227" t="n">
-        <v>-37.400837121237</v>
+        <v>-37.6316597490345</v>
       </c>
       <c r="AC227" t="n">
-        <v>9.4664891521827</v>
+        <v>9.74040240208549</v>
       </c>
       <c r="AD227" t="n">
-        <v>-13.113794317498</v>
+        <v>-10.2081997991299</v>
       </c>
       <c r="AE227" t="n">
-        <v>-3.64730516531535</v>
+        <v>-0.467797397044389</v>
       </c>
       <c r="AF227" t="n">
-        <v>-72.7611896904654</v>
+        <v>-69.9695297388301</v>
       </c>
       <c r="AG227" t="n">
-        <v>-18.5332265470615</v>
+        <v>-17.863837343984</v>
       </c>
     </row>
     <row r="228">
@@ -24109,25 +24109,25 @@
         <v>0</v>
       </c>
       <c r="H228" t="n">
-        <v>7.34102095684907</v>
+        <v>7.47914827160228</v>
       </c>
       <c r="I228" t="n">
-        <v>3.82586097335673</v>
+        <v>3.89799988312799</v>
       </c>
       <c r="J228" t="n">
-        <v>0.192008468477482</v>
+        <v>0.202965081576535</v>
       </c>
       <c r="K228" t="n">
         <v>0</v>
       </c>
       <c r="L228" t="n">
-        <v>0.0683531961042187</v>
+        <v>0.0722943589185927</v>
       </c>
       <c r="M228" t="n">
-        <v>-6.27170976280022</v>
+        <v>-6.36084953430071</v>
       </c>
       <c r="N228" t="n">
-        <v>-0.639171165395635</v>
+        <v>-0.648367418331776</v>
       </c>
       <c r="O228" t="n">
         <v>0</v>
@@ -24139,31 +24139,31 @@
         <v>0</v>
       </c>
       <c r="R228" t="n">
-        <v>-0.0504894757300376</v>
+        <v>-0.0514785550967738</v>
       </c>
       <c r="S228" t="n">
-        <v>-0.0599565730315564</v>
+        <v>-0.0624248395369921</v>
       </c>
       <c r="T228" t="n">
-        <v>-0.00280853422538725</v>
+        <v>-0.00282161942035962</v>
       </c>
       <c r="U228" t="n">
-        <v>-0.00660057160309517</v>
+        <v>-0.00668771367451321</v>
       </c>
       <c r="V228" t="n">
-        <v>-0.00568609239530368</v>
+        <v>-0.00575133510412946</v>
       </c>
       <c r="W228" t="n">
-        <v>-0.00599725402969195</v>
+        <v>-0.0061155612675597</v>
       </c>
       <c r="X228" t="n">
-        <v>-0.000249679355496173</v>
+        <v>-0.00025475012858761</v>
       </c>
       <c r="Y228" t="n">
-        <v>-5.00161548367288</v>
+        <v>-1.93541321531867</v>
       </c>
       <c r="Z228" t="n">
-        <v>-0.943381106587583</v>
+        <v>-0.956813049576864</v>
       </c>
       <c r="AA228" t="n">
         <v>0</v>
@@ -24172,19 +24172,19 @@
         <v>0</v>
       </c>
       <c r="AC228" t="n">
-        <v>11.4272435947875</v>
+        <v>11.6524075952254</v>
       </c>
       <c r="AD228" t="n">
-        <v>-12.9876656988269</v>
+        <v>-10.0369775917569</v>
       </c>
       <c r="AE228" t="n">
-        <v>-1.56042210403939</v>
+        <v>1.61543000346846</v>
       </c>
       <c r="AF228" t="n">
-        <v>-1.56042210403939</v>
+        <v>1.61543000346846</v>
       </c>
       <c r="AG228" t="n">
-        <v>-18.8177481496875</v>
+        <v>-17.3476884456007</v>
       </c>
     </row>
     <row r="229">
@@ -24210,25 +24210,25 @@
         <v>0</v>
       </c>
       <c r="H229" t="n">
-        <v>3.58949869709541</v>
+        <v>3.69116839388554</v>
       </c>
       <c r="I229" t="n">
-        <v>1.87937445055225</v>
+        <v>1.93251089510046</v>
       </c>
       <c r="J229" t="n">
-        <v>0.194121453611744</v>
+        <v>0.204021192136023</v>
       </c>
       <c r="K229" t="n">
         <v>0</v>
       </c>
       <c r="L229" t="n">
-        <v>0.0746267719807314</v>
+        <v>0.0781911247571371</v>
       </c>
       <c r="M229" t="n">
-        <v>-6.15576603601462</v>
+        <v>-6.21416477588445</v>
       </c>
       <c r="N229" t="n">
-        <v>-0.640332312065784</v>
+        <v>-0.64639407091655</v>
       </c>
       <c r="O229" t="n">
         <v>0</v>
@@ -24240,31 +24240,31 @@
         <v>0</v>
       </c>
       <c r="R229" t="n">
-        <v>-0.0468912806008519</v>
+        <v>-0.0476290650157223</v>
       </c>
       <c r="S229" t="n">
-        <v>-0.0553339920296613</v>
+        <v>-0.0574856453200442</v>
       </c>
       <c r="T229" t="n">
-        <v>-0.000296672217922851</v>
+        <v>-0.000296368724383302</v>
       </c>
       <c r="U229" t="n">
-        <v>-0.00299017072129983</v>
+        <v>-0.00304505368416158</v>
       </c>
       <c r="V229" t="n">
-        <v>-0.00315015642979454</v>
+        <v>-0.00318774760838464</v>
       </c>
       <c r="W229" t="n">
-        <v>-0.00560632495008648</v>
+        <v>-0.00569477124041224</v>
       </c>
       <c r="X229" t="n">
-        <v>-0.000246126469492257</v>
+        <v>-0.000249952018310104</v>
       </c>
       <c r="Y229" t="n">
-        <v>-4.98875249625449</v>
+        <v>-1.90967860308489</v>
       </c>
       <c r="Z229" t="n">
-        <v>-0.935283001405661</v>
+        <v>-0.944090591852492</v>
       </c>
       <c r="AA229" t="n">
         <v>0</v>
@@ -24273,19 +24273,19 @@
         <v>0</v>
       </c>
       <c r="AC229" t="n">
-        <v>5.73762137324014</v>
+        <v>5.90589160587917</v>
       </c>
       <c r="AD229" t="n">
-        <v>-12.8346485691597</v>
+        <v>-9.8319166453498</v>
       </c>
       <c r="AE229" t="n">
-        <v>-7.09702719591952</v>
+        <v>-3.92602503947063</v>
       </c>
       <c r="AF229" t="n">
-        <v>-7.09702719591952</v>
+        <v>-3.92602503947063</v>
       </c>
       <c r="AG229" t="n">
-        <v>-20.4592946834256</v>
+        <v>-18.1869547372569</v>
       </c>
     </row>
     <row r="230">
@@ -24311,25 +24311,25 @@
         <v>0</v>
       </c>
       <c r="H230" t="n">
-        <v>3.59482671248795</v>
+        <v>3.67898526427803</v>
       </c>
       <c r="I230" t="n">
-        <v>1.87161614428843</v>
+        <v>1.91558481981979</v>
       </c>
       <c r="J230" t="n">
-        <v>0.201719884929916</v>
+        <v>0.210642988137611</v>
       </c>
       <c r="K230" t="n">
         <v>0</v>
       </c>
       <c r="L230" t="n">
-        <v>0.0750185918376533</v>
+        <v>0.0782091184917739</v>
       </c>
       <c r="M230" t="n">
-        <v>-6.19421666045563</v>
+        <v>-6.2233653994001</v>
       </c>
       <c r="N230" t="n">
-        <v>-0.641594706452758</v>
+        <v>-0.644613922219932</v>
       </c>
       <c r="O230" t="n">
         <v>0</v>
@@ -24341,31 +24341,31 @@
         <v>0</v>
       </c>
       <c r="R230" t="n">
-        <v>-0.0433750387633546</v>
+        <v>-0.04388804081668</v>
       </c>
       <c r="S230" t="n">
-        <v>-0.0500848040394384</v>
+        <v>-0.0519625805553657</v>
       </c>
       <c r="T230" t="n">
-        <v>-0.000292464280444016</v>
+        <v>-0.000290772093670924</v>
       </c>
       <c r="U230" t="n">
-        <v>-0.00131578199585016</v>
+        <v>-0.00135627825793918</v>
       </c>
       <c r="V230" t="n">
-        <v>-0.00177785492761094</v>
+        <v>-0.00180042581795246</v>
       </c>
       <c r="W230" t="n">
-        <v>-0.00519572632675305</v>
+        <v>-0.00525729602798994</v>
       </c>
       <c r="X230" t="n">
-        <v>-0.000242649783946854</v>
+        <v>-0.00024529579453769</v>
       </c>
       <c r="Y230" t="n">
-        <v>-4.97668487240074</v>
+        <v>-1.88463327271084</v>
       </c>
       <c r="Z230" t="n">
-        <v>-0.927344996192522</v>
+        <v>-0.931708895404838</v>
       </c>
       <c r="AA230" t="n">
         <v>0</v>
@@ -24374,19 +24374,19 @@
         <v>0</v>
       </c>
       <c r="AC230" t="n">
-        <v>5.74318133354395</v>
+        <v>5.8834221907272</v>
       </c>
       <c r="AD230" t="n">
-        <v>-12.8421255556191</v>
+        <v>-9.78912217909984</v>
       </c>
       <c r="AE230" t="n">
-        <v>-7.0989442220751</v>
+        <v>-3.90569998837265</v>
       </c>
       <c r="AF230" t="n">
-        <v>-7.0989442220751</v>
+        <v>-3.90569998837265</v>
       </c>
       <c r="AG230" t="n">
-        <v>-22.1293958031249</v>
+        <v>-19.0464561908012</v>
       </c>
     </row>
     <row r="231">
@@ -24412,19 +24412,19 @@
         <v>0</v>
       </c>
       <c r="H231" t="n">
-        <v>3.56797560038849</v>
+        <v>3.6349763090684</v>
       </c>
       <c r="I231" t="n">
-        <v>1.86366959291199</v>
+        <v>1.89870463611531</v>
       </c>
       <c r="J231" t="n">
-        <v>0.203512880998237</v>
+        <v>0.211458115264035</v>
       </c>
       <c r="K231" t="n">
         <v>0</v>
       </c>
       <c r="L231" t="n">
-        <v>0.0754912038313918</v>
+        <v>0.0783185251358729</v>
       </c>
       <c r="M231" t="n">
         <v>0</v>
@@ -24442,25 +24442,25 @@
         <v>0</v>
       </c>
       <c r="R231" t="n">
-        <v>-0.0257943200696954</v>
+        <v>-0.0261020994028258</v>
       </c>
       <c r="S231" t="n">
-        <v>-0.0426156321678845</v>
+        <v>-0.0442518267126678</v>
       </c>
       <c r="T231" t="n">
-        <v>-0.000288415037551126</v>
+        <v>-0.000285357584419228</v>
       </c>
       <c r="U231" t="n">
-        <v>-0.000993036064356082</v>
+        <v>-0.00102721741261374</v>
       </c>
       <c r="V231" t="n">
-        <v>-0.00150650320584166</v>
+        <v>-0.00152065689196695</v>
       </c>
       <c r="W231" t="n">
-        <v>-0.00308802944272969</v>
+        <v>-0.00312501588885578</v>
       </c>
       <c r="X231" t="n">
-        <v>-0.0000808382464693936</v>
+        <v>-0.0000823369980046373</v>
       </c>
       <c r="Y231" t="n">
         <v>0</v>
@@ -24475,19 +24475,19 @@
         <v>0</v>
       </c>
       <c r="AC231" t="n">
-        <v>5.71064927813011</v>
+        <v>5.82345758558363</v>
       </c>
       <c r="AD231" t="n">
-        <v>-0.0743667742345278</v>
+        <v>-0.0763945108913539</v>
       </c>
       <c r="AE231" t="n">
-        <v>5.63628250389558</v>
+        <v>5.74706307469227</v>
       </c>
       <c r="AF231" t="n">
-        <v>5.63628250389558</v>
+        <v>5.74706307469227</v>
       </c>
       <c r="AG231" t="n">
-        <v>-2.53002775453461</v>
+        <v>-0.117307987420642</v>
       </c>
     </row>
     <row r="232">
@@ -24513,19 +24513,19 @@
         <v>0</v>
       </c>
       <c r="H232" t="n">
-        <v>3.54271794870323</v>
+        <v>3.59270603794707</v>
       </c>
       <c r="I232" t="n">
-        <v>1.85560567102224</v>
+        <v>1.88175430149973</v>
       </c>
       <c r="J232" t="n">
-        <v>0.205447474209381</v>
+        <v>0.212404202286098</v>
       </c>
       <c r="K232" t="n">
         <v>0</v>
       </c>
       <c r="L232" t="n">
-        <v>0.0755660779655674</v>
+        <v>0.0780272491649796</v>
       </c>
       <c r="M232" t="n">
         <v>0</v>
@@ -24543,25 +24543,25 @@
         <v>0</v>
       </c>
       <c r="R232" t="n">
-        <v>-0.0142221840007382</v>
+        <v>-0.0144077486405538</v>
       </c>
       <c r="S232" t="n">
-        <v>-0.0424678318154382</v>
+        <v>-0.0438971540573117</v>
       </c>
       <c r="T232" t="n">
-        <v>-0.000284477599182361</v>
+        <v>-0.000280082191413928</v>
       </c>
       <c r="U232" t="n">
-        <v>-0.000983210364684009</v>
+        <v>-0.00101258848718434</v>
       </c>
       <c r="V232" t="n">
-        <v>-0.00125123560161194</v>
+        <v>-0.0012582682069139</v>
       </c>
       <c r="W232" t="n">
-        <v>-0.00170545512477903</v>
+        <v>-0.00172780972816472</v>
       </c>
       <c r="X232" t="n">
-        <v>-0.0000797243746749887</v>
+        <v>-0.0000808377625138823</v>
       </c>
       <c r="Y232" t="n">
         <v>0</v>
@@ -24576,19 +24576,19 @@
         <v>0</v>
       </c>
       <c r="AC232" t="n">
-        <v>5.67933717190042</v>
+        <v>5.76489179089788</v>
       </c>
       <c r="AD232" t="n">
-        <v>-0.0609941188811087</v>
+        <v>-0.0626644890740562</v>
       </c>
       <c r="AE232" t="n">
-        <v>5.61834305301932</v>
+        <v>5.70222730182382</v>
       </c>
       <c r="AF232" t="n">
-        <v>5.61834305301932</v>
+        <v>5.70222730182382</v>
       </c>
       <c r="AG232" t="n">
-        <v>-0.735336465269932</v>
+        <v>0.904391337168198</v>
       </c>
     </row>
     <row r="233">
@@ -24614,19 +24614,19 @@
         <v>0</v>
       </c>
       <c r="H233" t="n">
-        <v>3.51798426581115</v>
+        <v>3.55127046865678</v>
       </c>
       <c r="I233" t="n">
-        <v>1.84737334931225</v>
+        <v>1.86477390521435</v>
       </c>
       <c r="J233" t="n">
-        <v>0.206557993611421</v>
+        <v>0.212540978085828</v>
       </c>
       <c r="K233" t="n">
         <v>0</v>
       </c>
       <c r="L233" t="n">
-        <v>0.0750701787467338</v>
+        <v>0.0771733197159231</v>
       </c>
       <c r="M233" t="n">
         <v>0</v>
@@ -24644,25 +24644,25 @@
         <v>0</v>
       </c>
       <c r="R233" t="n">
-        <v>-0.0140270396725678</v>
+        <v>-0.0141455741364896</v>
       </c>
       <c r="S233" t="n">
-        <v>-0.0435622537872699</v>
+        <v>-0.0447903056036093</v>
       </c>
       <c r="T233" t="n">
-        <v>0.000195375965316679</v>
+        <v>0.000201101794547248</v>
       </c>
       <c r="U233" t="n">
-        <v>-0.000982897253508742</v>
+        <v>-0.00100762032322826</v>
       </c>
       <c r="V233" t="n">
-        <v>-0.000243400907868585</v>
+        <v>-0.000244548204408272</v>
       </c>
       <c r="W233" t="n">
-        <v>-0.00169417961741289</v>
+        <v>-0.00170849615728338</v>
       </c>
       <c r="X233" t="n">
-        <v>-0.0000786302761828208</v>
+        <v>-0.0000793678239583342</v>
       </c>
       <c r="Y233" t="n">
         <v>0</v>
@@ -24677,19 +24677,19 @@
         <v>0</v>
       </c>
       <c r="AC233" t="n">
-        <v>5.64698578748156</v>
+        <v>5.70575867167288</v>
       </c>
       <c r="AD233" t="n">
-        <v>-0.0603930255494941</v>
+        <v>-0.0617748104544299</v>
       </c>
       <c r="AE233" t="n">
-        <v>5.58659276193206</v>
+        <v>5.64398386121845</v>
       </c>
       <c r="AF233" t="n">
-        <v>5.58659276193206</v>
+        <v>5.64398386121845</v>
       </c>
       <c r="AG233" t="n">
-        <v>2.43556852419296</v>
+        <v>3.29689356234047</v>
       </c>
     </row>
     <row r="234">
@@ -24715,19 +24715,19 @@
         <v>0</v>
       </c>
       <c r="H234" t="n">
-        <v>3.53049854837285</v>
+        <v>3.54722251898612</v>
       </c>
       <c r="I234" t="n">
-        <v>1.83729310096856</v>
+        <v>1.84599635786205</v>
       </c>
       <c r="J234" t="n">
-        <v>0.207682823870142</v>
+        <v>0.212698222991494</v>
       </c>
       <c r="K234" t="n">
         <v>0</v>
       </c>
       <c r="L234" t="n">
-        <v>0.0746923475182203</v>
+        <v>0.0764437491025072</v>
       </c>
       <c r="M234" t="n">
         <v>0</v>
@@ -24745,25 +24745,25 @@
         <v>0</v>
       </c>
       <c r="R234" t="n">
-        <v>-0.0110786958734571</v>
+        <v>-0.0111311756526391</v>
       </c>
       <c r="S234" t="n">
-        <v>-0.0425555718373158</v>
+        <v>-0.0435795230456598</v>
       </c>
       <c r="T234" t="n">
-        <v>0.000192670439824647</v>
+        <v>0.000197481144560533</v>
       </c>
       <c r="U234" t="n">
-        <v>-0.000992460186024399</v>
+        <v>-0.00101257451916756</v>
       </c>
       <c r="V234" t="n">
         <v>0</v>
       </c>
       <c r="W234" t="n">
-        <v>-0.00133807996373131</v>
+        <v>-0.00134441844813657</v>
       </c>
       <c r="X234" t="n">
-        <v>-0.0000775508711141996</v>
+        <v>-0.0000779182295684739</v>
       </c>
       <c r="Y234" t="n">
         <v>0</v>
@@ -24778,19 +24778,19 @@
         <v>0</v>
       </c>
       <c r="AC234" t="n">
-        <v>5.65016682072977</v>
+        <v>5.68236084894217</v>
       </c>
       <c r="AD234" t="n">
-        <v>-0.0558496882918182</v>
+        <v>-0.056948128750611</v>
       </c>
       <c r="AE234" t="n">
-        <v>5.59431713243795</v>
+        <v>5.62541272019156</v>
       </c>
       <c r="AF234" t="n">
-        <v>5.59431713243795</v>
+        <v>5.62541272019156</v>
       </c>
       <c r="AG234" t="n">
-        <v>5.60888386282123</v>
+        <v>5.67967173948152</v>
       </c>
     </row>
     <row r="235">
@@ -24822,13 +24822,13 @@
         <v>0</v>
       </c>
       <c r="J235" t="n">
-        <v>0.208901120628369</v>
+        <v>0.212942315570546</v>
       </c>
       <c r="K235" t="n">
         <v>0</v>
       </c>
       <c r="L235" t="n">
-        <v>0.0743339188759051</v>
+        <v>0.0757348270278107</v>
       </c>
       <c r="M235" t="n">
         <v>0</v>
@@ -24849,13 +24849,13 @@
         <v>0</v>
       </c>
       <c r="S235" t="n">
-        <v>-0.0320677894322871</v>
+        <v>-0.0328921109306041</v>
       </c>
       <c r="T235" t="n">
-        <v>0.000190064068152045</v>
+        <v>0.000193971364641815</v>
       </c>
       <c r="U235" t="n">
-        <v>-0.000582408435796675</v>
+        <v>-0.000597858145735165</v>
       </c>
       <c r="V235" t="n">
         <v>0</v>
@@ -24879,19 +24879,19 @@
         <v>0</v>
       </c>
       <c r="AC235" t="n">
-        <v>0.283235039504274</v>
+        <v>0.288677142598356</v>
       </c>
       <c r="AD235" t="n">
-        <v>-0.0324601337999317</v>
+        <v>-0.0332959977116974</v>
       </c>
       <c r="AE235" t="n">
-        <v>0.250774905704343</v>
+        <v>0.255381144886659</v>
       </c>
       <c r="AF235" t="n">
-        <v>0.250774905704343</v>
+        <v>0.255381144886659</v>
       </c>
       <c r="AG235" t="n">
-        <v>4.26250696327342</v>
+        <v>4.30675125703011</v>
       </c>
     </row>
     <row r="236">
@@ -24923,13 +24923,13 @@
         <v>0</v>
       </c>
       <c r="J236" t="n">
-        <v>0.210090249656128</v>
+        <v>0.213133883917379</v>
       </c>
       <c r="K236" t="n">
         <v>0</v>
       </c>
       <c r="L236" t="n">
-        <v>0.0737190428986672</v>
+        <v>0.0747650089411367</v>
       </c>
       <c r="M236" t="n">
         <v>0</v>
@@ -24950,13 +24950,13 @@
         <v>0</v>
       </c>
       <c r="S236" t="n">
-        <v>-0.0318421166831904</v>
+        <v>-0.0325131794793199</v>
       </c>
       <c r="T236" t="n">
-        <v>0.00018744028906882</v>
+        <v>0.000190439834478947</v>
       </c>
       <c r="U236" t="n">
-        <v>-0.000583462254165791</v>
+        <v>-0.000596128215914088</v>
       </c>
       <c r="V236" t="n">
         <v>0</v>
@@ -24980,19 +24980,19 @@
         <v>0</v>
       </c>
       <c r="AC236" t="n">
-        <v>0.283809292554795</v>
+        <v>0.287898892858515</v>
       </c>
       <c r="AD236" t="n">
-        <v>-0.0322381386482874</v>
+        <v>-0.0329188678607551</v>
       </c>
       <c r="AE236" t="n">
-        <v>0.251571153906508</v>
+        <v>0.25498002499776</v>
       </c>
       <c r="AF236" t="n">
-        <v>0.251571153906508</v>
+        <v>0.25498002499776</v>
       </c>
       <c r="AG236" t="n">
-        <v>2.92081398849522</v>
+        <v>2.9449394378236</v>
       </c>
     </row>
     <row r="237">
@@ -25024,13 +25024,13 @@
         <v>0</v>
       </c>
       <c r="J237" t="n">
-        <v>0.211284270734589</v>
+        <v>0.21332052110136</v>
       </c>
       <c r="K237" t="n">
         <v>0</v>
       </c>
       <c r="L237" t="n">
-        <v>0.0727283511369669</v>
+        <v>0.0734208633555086</v>
       </c>
       <c r="M237" t="n">
         <v>0</v>
@@ -25051,13 +25051,13 @@
         <v>0</v>
       </c>
       <c r="S237" t="n">
-        <v>-0.0333073621121984</v>
+        <v>-0.0338254618496985</v>
       </c>
       <c r="T237" t="n">
-        <v>0.000438032242245689</v>
+        <v>0.000440132631366132</v>
       </c>
       <c r="U237" t="n">
-        <v>-0.000586800181445484</v>
+        <v>-0.000596662815721709</v>
       </c>
       <c r="V237" t="n">
         <v>0</v>
@@ -25081,19 +25081,19 @@
         <v>0</v>
       </c>
       <c r="AC237" t="n">
-        <v>0.284012621871556</v>
+        <v>0.286741384456868</v>
       </c>
       <c r="AD237" t="n">
-        <v>-0.0334561300513982</v>
+        <v>-0.0339819920340541</v>
       </c>
       <c r="AE237" t="n">
-        <v>0.250556491820158</v>
+        <v>0.252759392422814</v>
       </c>
       <c r="AF237" t="n">
-        <v>0.250556491820158</v>
+        <v>0.252759392422814</v>
       </c>
       <c r="AG237" t="n">
-        <v>1.58680492096724</v>
+        <v>1.59713332062469</v>
       </c>
     </row>
     <row r="238">
@@ -25125,13 +25125,13 @@
         <v>0</v>
       </c>
       <c r="J238" t="n">
-        <v>0.21248178173747</v>
+        <v>0.21350434096293</v>
       </c>
       <c r="K238" t="n">
         <v>0</v>
       </c>
       <c r="L238" t="n">
-        <v>0.0713946820979732</v>
+        <v>0.0717382658642193</v>
       </c>
       <c r="M238" t="n">
         <v>0</v>
@@ -25152,13 +25152,13 @@
         <v>0</v>
       </c>
       <c r="S238" t="n">
-        <v>-0.0325953617878963</v>
+        <v>-0.0329535507630979</v>
       </c>
       <c r="T238" t="n">
         <v>0</v>
       </c>
       <c r="U238" t="n">
-        <v>-0.000491184148601089</v>
+        <v>-0.000498229107606513</v>
       </c>
       <c r="V238" t="n">
         <v>0</v>
@@ -25182,19 +25182,19 @@
         <v>0</v>
       </c>
       <c r="AC238" t="n">
-        <v>0.283876463835443</v>
+        <v>0.285242606827149</v>
       </c>
       <c r="AD238" t="n">
-        <v>-0.0330865459364974</v>
+        <v>-0.0334517798707044</v>
       </c>
       <c r="AE238" t="n">
-        <v>0.250789917898946</v>
+        <v>0.251790826956445</v>
       </c>
       <c r="AF238" t="n">
-        <v>0.250789917898946</v>
+        <v>0.251790826956445</v>
       </c>
       <c r="AG238" t="n">
-        <v>0.25092311733249</v>
+        <v>0.253727847315912</v>
       </c>
     </row>
     <row r="239">
@@ -25253,13 +25253,13 @@
         <v>0</v>
       </c>
       <c r="S239" t="n">
-        <v>-0.0102384425769539</v>
+        <v>-0.0104390726378308</v>
       </c>
       <c r="T239" t="n">
         <v>0</v>
       </c>
       <c r="U239" t="n">
-        <v>-0.00038886337800323</v>
+        <v>-0.000393528371012856</v>
       </c>
       <c r="V239" t="n">
         <v>0</v>
@@ -25286,16 +25286,16 @@
         <v>0</v>
       </c>
       <c r="AD239" t="n">
-        <v>-0.0106273059549571</v>
+        <v>-0.0108326010088437</v>
       </c>
       <c r="AE239" t="n">
-        <v>-0.0106273059549571</v>
+        <v>-0.0108326010088437</v>
       </c>
       <c r="AF239" t="n">
-        <v>-0.0106273059549571</v>
+        <v>-0.0108326010088437</v>
       </c>
       <c r="AG239" t="n">
-        <v>0.185572564417665</v>
+        <v>0.187174410842036</v>
       </c>
     </row>
     <row r="240">
@@ -25354,13 +25354,13 @@
         <v>0</v>
       </c>
       <c r="S240" t="n">
-        <v>-0.0101974863743186</v>
+        <v>-0.010348254093353</v>
       </c>
       <c r="T240" t="n">
         <v>0</v>
       </c>
       <c r="U240" t="n">
-        <v>-0.000288816249438213</v>
+        <v>-0.00029159818734561</v>
       </c>
       <c r="V240" t="n">
         <v>0</v>
@@ -25387,16 +25387,16 @@
         <v>0</v>
       </c>
       <c r="AD240" t="n">
-        <v>-0.0104863026237568</v>
+        <v>-0.0106398522806986</v>
       </c>
       <c r="AE240" t="n">
-        <v>-0.0104863026237568</v>
+        <v>-0.0106398522806986</v>
       </c>
       <c r="AF240" t="n">
-        <v>-0.0104863026237568</v>
+        <v>-0.0106398522806986</v>
       </c>
       <c r="AG240" t="n">
-        <v>0.120058200285099</v>
+        <v>0.120769441522422</v>
       </c>
     </row>
     <row r="241">
@@ -25455,13 +25455,13 @@
         <v>0</v>
       </c>
       <c r="S241" t="n">
-        <v>-0.0106048896560545</v>
+        <v>-0.0107062066615528</v>
       </c>
       <c r="T241" t="n">
         <v>0</v>
       </c>
       <c r="U241" t="n">
-        <v>-0.000191064728518691</v>
+        <v>-0.000192450503772596</v>
       </c>
       <c r="V241" t="n">
         <v>0</v>
@@ -25488,16 +25488,16 @@
         <v>0</v>
       </c>
       <c r="AD241" t="n">
-        <v>-0.0107959543845732</v>
+        <v>-0.0108986571653254</v>
       </c>
       <c r="AE241" t="n">
-        <v>-0.0107959543845732</v>
+        <v>-0.0108986571653254</v>
       </c>
       <c r="AF241" t="n">
-        <v>-0.0107959543845732</v>
+        <v>-0.0108986571653254</v>
       </c>
       <c r="AG241" t="n">
-        <v>0.0547200887339165</v>
+        <v>0.0548549291253868</v>
       </c>
     </row>
     <row r="242">
@@ -25556,13 +25556,13 @@
         <v>0</v>
       </c>
       <c r="S242" t="n">
-        <v>-0.0103368301256772</v>
+        <v>-0.0103867386457179</v>
       </c>
       <c r="T242" t="n">
         <v>0</v>
       </c>
       <c r="U242" t="n">
-        <v>-0.0000955769759929711</v>
+        <v>-0.0000960384429382324</v>
       </c>
       <c r="V242" t="n">
         <v>0</v>
@@ -25589,16 +25589,16 @@
         <v>0</v>
       </c>
       <c r="AD242" t="n">
-        <v>-0.0104324071016701</v>
+        <v>-0.0104827770886562</v>
       </c>
       <c r="AE242" t="n">
-        <v>-0.0104324071016701</v>
+        <v>-0.0104827770886562</v>
       </c>
       <c r="AF242" t="n">
-        <v>-0.0104324071016701</v>
+        <v>-0.0104827770886562</v>
       </c>
       <c r="AG242" t="n">
-        <v>-0.0105854925162375</v>
+        <v>-0.0107134718858884</v>
       </c>
     </row>
     <row r="243">
@@ -25699,7 +25699,7 @@
         <v>0</v>
       </c>
       <c r="AG243" t="n">
-        <v>-0.00792866602749823</v>
+        <v>-0.00800532163367752</v>
       </c>
     </row>
     <row r="244">
@@ -25800,7 +25800,7 @@
         <v>0</v>
       </c>
       <c r="AG244" t="n">
-        <v>-0.00530709037155903</v>
+        <v>-0.00534535856350286</v>
       </c>
     </row>
     <row r="245">
@@ -25901,7 +25901,7 @@
         <v>0</v>
       </c>
       <c r="AG245" t="n">
-        <v>-0.00260810177541573</v>
+        <v>-0.0026206942721715</v>
       </c>
     </row>
     <row r="246">
@@ -26002,7 +26002,7 @@
         <v>0</v>
       </c>
       <c r="AG246" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="247">
@@ -26103,7 +26103,7 @@
         <v>0</v>
       </c>
       <c r="AG247" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="248">
@@ -26204,7 +26204,7 @@
         <v>0</v>
       </c>
       <c r="AG248" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="249">
@@ -26305,7 +26305,7 @@
         <v>0</v>
       </c>
       <c r="AG249" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="250">
@@ -26406,7 +26406,7 @@
         <v>0</v>
       </c>
       <c r="AG250" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="251">
@@ -26507,7 +26507,7 @@
         <v>0</v>
       </c>
       <c r="AG251" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="252">
@@ -26608,7 +26608,7 @@
         <v>0</v>
       </c>
       <c r="AG252" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="253">
@@ -26709,7 +26709,7 @@
         <v>0</v>
       </c>
       <c r="AG253" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="254">
@@ -26810,7 +26810,7 @@
         <v>0</v>
       </c>
       <c r="AG254" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="255">
@@ -26911,7 +26911,7 @@
         <v>0</v>
       </c>
       <c r="AG255" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="256">
@@ -27012,7 +27012,7 @@
         <v>0</v>
       </c>
       <c r="AG256" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="257">
@@ -27113,7 +27113,7 @@
         <v>0</v>
       </c>
       <c r="AG257" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="258">
@@ -27214,7 +27214,7 @@
         <v>0</v>
       </c>
       <c r="AG258" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="259">
@@ -27315,7 +27315,7 @@
         <v>0</v>
       </c>
       <c r="AG259" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
     <row r="260">
@@ -27416,7 +27416,7 @@
         <v>0</v>
       </c>
       <c r="AG260" t="n">
-        <v>0.00000000000000180151032980191</v>
+        <v>-0.00000000000000746061198930725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data: run FIM, and results now match the original
</commit_message>
<xml_diff>
--- a/results/07-2024/beta/contributions-07-2024.xlsx
+++ b/results/07-2024/beta/contributions-07-2024.xlsx
@@ -770,10 +770,10 @@
     <t xml:space="preserve">2024 Q2</t>
   </si>
   <si>
+    <t xml:space="preserve">2024 Q3</t>
+  </si>
+  <si>
     <t xml:space="preserve">projection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 Q3</t>
   </si>
   <si>
     <t xml:space="preserve">2024 Q4</t>
@@ -23182,43 +23182,43 @@
         <v>251</v>
       </c>
       <c r="B219" t="s">
-        <v>252</v>
+        <v>34</v>
       </c>
       <c r="C219" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D219" t="n">
-        <v>0.0279492709152113</v>
+        <v>0.115426641109984</v>
       </c>
       <c r="E219" t="n">
-        <v>-0.00915388060511806</v>
+        <v>0.0213495782472853</v>
       </c>
       <c r="F219" t="n">
-        <v>-0.0165627919074172</v>
+        <v>-0.00841229468813802</v>
       </c>
       <c r="G219" t="n">
-        <v>-0.183252705496367</v>
+        <v>0.0584823625448953</v>
       </c>
       <c r="H219" t="n">
-        <v>0.204480619338558</v>
+        <v>0.194479203432638</v>
       </c>
       <c r="I219" t="n">
-        <v>0.190804110337713</v>
+        <v>0.185561555981642</v>
       </c>
       <c r="J219" t="n">
-        <v>-0.0531988343104604</v>
+        <v>-0.0534865745908126</v>
       </c>
       <c r="K219" t="n">
-        <v>0.0343320274759174</v>
+        <v>0.0366848996418076</v>
       </c>
       <c r="L219" t="n">
-        <v>-0.0231228664014136</v>
+        <v>-0.0232300873829199</v>
       </c>
       <c r="M219" t="n">
-        <v>0.0794503265832219</v>
+        <v>0.0882092651530837</v>
       </c>
       <c r="N219" t="n">
-        <v>0.0478523737781044</v>
+        <v>-0.012591686958121</v>
       </c>
       <c r="O219" t="n">
         <v>0</v>
@@ -23227,156 +23227,156 @@
         <v>-0.104929405936357</v>
       </c>
       <c r="Q219" t="n">
-        <v>0.000194141410154632</v>
+        <v>-0.00065483910574253</v>
       </c>
       <c r="R219" t="n">
-        <v>-0.00129223973278812</v>
+        <v>-0.000356899088675943</v>
       </c>
       <c r="S219" t="n">
-        <v>-0.294446895031987</v>
+        <v>-0.293399973248863</v>
       </c>
       <c r="T219" t="n">
-        <v>-0.0176894198471784</v>
+        <v>-0.0176883812429932</v>
       </c>
       <c r="U219" t="n">
-        <v>-0.0357568441307092</v>
+        <v>-0.0357529054240686</v>
       </c>
       <c r="V219" t="n">
-        <v>-0.0488511740515331</v>
+        <v>-0.0488351118285673</v>
       </c>
       <c r="W219" t="n">
-        <v>-0.0931683179086759</v>
+        <v>-0.0931584967077159</v>
       </c>
       <c r="X219" t="n">
-        <v>-0.00261741163164872</v>
+        <v>-0.0021264662695237</v>
       </c>
       <c r="Y219" t="n">
-        <v>-0.158486103223233</v>
+        <v>-0.151728603424376</v>
       </c>
       <c r="Z219" t="n">
-        <v>0.110854636619516</v>
+        <v>0.112152881864364</v>
       </c>
       <c r="AA219" t="n">
-        <v>0.00223259840267611</v>
+        <v>0.128363924669132</v>
       </c>
       <c r="AB219" t="n">
-        <v>-0.157536032983832</v>
+        <v>0.045545078985748</v>
       </c>
       <c r="AC219" t="n">
-        <v>0.353295056440314</v>
+        <v>0.340008997082355</v>
       </c>
       <c r="AD219" t="n">
-        <v>-0.518886333103112</v>
+        <v>-0.560860622217557</v>
       </c>
       <c r="AE219" t="n">
-        <v>-0.165591276662798</v>
+        <v>-0.220851625135203</v>
       </c>
       <c r="AF219" t="n">
-        <v>-0.320894711243953</v>
+        <v>-0.0469426214803228</v>
       </c>
       <c r="AG219" t="n">
-        <v>0.149066737256533</v>
+        <v>0.217554759697441</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
+        <v>252</v>
+      </c>
+      <c r="B220" t="s">
         <v>253</v>
       </c>
-      <c r="B220" t="s">
-        <v>252</v>
-      </c>
       <c r="C220" t="n">
         <v>0</v>
       </c>
       <c r="D220" t="n">
-        <v>-0.313587498166553</v>
+        <v>-0.313908433215255</v>
       </c>
       <c r="E220" t="n">
-        <v>-0.000868263211866176</v>
+        <v>-0.000869151819026267</v>
       </c>
       <c r="F220" t="n">
-        <v>-0.0117473732878433</v>
+        <v>-0.0117593959094092</v>
       </c>
       <c r="G220" t="n">
-        <v>-0.0651536074647197</v>
+        <v>-0.0652202876618162</v>
       </c>
       <c r="H220" t="n">
-        <v>0.303143948086791</v>
+        <v>0.293578542527128</v>
       </c>
       <c r="I220" t="n">
-        <v>0.0978813610311459</v>
+        <v>0.092804904346207</v>
       </c>
       <c r="J220" t="n">
-        <v>-0.0596759361881238</v>
+        <v>-0.0600211324375351</v>
       </c>
       <c r="K220" t="n">
-        <v>0.0329899161852774</v>
+        <v>0.0330236790757609</v>
       </c>
       <c r="L220" t="n">
-        <v>-0.0163866719464414</v>
+        <v>-0.0165093152916424</v>
       </c>
       <c r="M220" t="n">
-        <v>0.112658428659887</v>
+        <v>0.121422525392554</v>
       </c>
       <c r="N220" t="n">
-        <v>0.0542407360954437</v>
+        <v>0.0556989552299827</v>
       </c>
       <c r="O220" t="n">
         <v>0</v>
       </c>
       <c r="P220" t="n">
-        <v>-0.101647463813208</v>
+        <v>-0.101751492940453</v>
       </c>
       <c r="Q220" t="n">
-        <v>-0.000463143029123872</v>
+        <v>-0.00032884297838877</v>
       </c>
       <c r="R220" t="n">
-        <v>-0.0000591389286745778</v>
+        <v>-0.000121490440341458</v>
       </c>
       <c r="S220" t="n">
-        <v>-0.264478372109838</v>
+        <v>-0.264810460233818</v>
       </c>
       <c r="T220" t="n">
-        <v>-0.0667863712509886</v>
+        <v>-0.0668536969243649</v>
       </c>
       <c r="U220" t="n">
-        <v>-0.0343544346411838</v>
+        <v>-0.0343868160365828</v>
       </c>
       <c r="V220" t="n">
-        <v>-0.0432124205683029</v>
+        <v>-0.04324316427257</v>
       </c>
       <c r="W220" t="n">
-        <v>-0.0548086501794876</v>
+        <v>-0.0548564999824933</v>
       </c>
       <c r="X220" t="n">
-        <v>-0.000487343058014932</v>
+        <v>-0.000558510102538113</v>
       </c>
       <c r="Y220" t="n">
-        <v>0.0691635470173543</v>
+        <v>0.0759068582255419</v>
       </c>
       <c r="Z220" t="n">
-        <v>0.059904249385294</v>
+        <v>0.0612474775922516</v>
       </c>
       <c r="AA220" t="n">
-        <v>-0.326203134666263</v>
+        <v>-0.32653698094369</v>
       </c>
       <c r="AB220" t="n">
-        <v>-0.0525379709650102</v>
+        <v>-0.0525917399333808</v>
       </c>
       <c r="AC220" t="n">
-        <v>0.357952617168649</v>
+        <v>0.342876678219918</v>
       </c>
       <c r="AD220" t="n">
-        <v>-0.270330376420844</v>
+        <v>-0.25263515747122</v>
       </c>
       <c r="AE220" t="n">
-        <v>0.0876222407478053</v>
+        <v>0.0902415207486977</v>
       </c>
       <c r="AF220" t="n">
-        <v>-0.291118864883468</v>
+        <v>-0.288887200128373</v>
       </c>
       <c r="AG220" t="n">
-        <v>-0.0668476306972017</v>
+        <v>0.0021983079324796</v>
       </c>
     </row>
     <row r="221">
@@ -23384,100 +23384,100 @@
         <v>254</v>
       </c>
       <c r="B221" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C221" t="n">
         <v>0</v>
       </c>
       <c r="D221" t="n">
-        <v>-0.0305030066406614</v>
+        <v>-0.0305342243517596</v>
       </c>
       <c r="E221" t="n">
-        <v>0.0039435964146431</v>
+        <v>0.0039476324119797</v>
       </c>
       <c r="F221" t="n">
-        <v>0.0106466587806725</v>
+        <v>0.0106575548973042</v>
       </c>
       <c r="G221" t="n">
-        <v>-0.0634619784856173</v>
+        <v>-0.0635269274178134</v>
       </c>
       <c r="H221" t="n">
-        <v>0.210554810667858</v>
+        <v>0.205885381236198</v>
       </c>
       <c r="I221" t="n">
-        <v>0.0685581178825413</v>
+        <v>0.0660677002717437</v>
       </c>
       <c r="J221" t="n">
-        <v>-0.0528276164894034</v>
+        <v>-0.0531627596080454</v>
       </c>
       <c r="K221" t="n">
-        <v>0.0314804078741684</v>
+        <v>0.0315126258876201</v>
       </c>
       <c r="L221" t="n">
-        <v>0.000592764259184759</v>
+        <v>0.000488632608747897</v>
       </c>
       <c r="M221" t="n">
-        <v>0.108310661610859</v>
+        <v>0.116977637354586</v>
       </c>
       <c r="N221" t="n">
-        <v>0.0630494703994884</v>
+        <v>0.0645016747369498</v>
       </c>
       <c r="O221" t="n">
         <v>0</v>
       </c>
       <c r="P221" t="n">
-        <v>-0.0997020018394068</v>
+        <v>-0.0998040399212916</v>
       </c>
       <c r="Q221" t="n">
-        <v>-0.00021724290465523</v>
+        <v>-0.000168407278836746</v>
       </c>
       <c r="R221" t="n">
-        <v>-0.00218484481891573</v>
+        <v>-0.0021686504319439</v>
       </c>
       <c r="S221" t="n">
-        <v>-0.107950790264199</v>
+        <v>-0.108039786312362</v>
       </c>
       <c r="T221" t="n">
-        <v>-0.029004087876285</v>
+        <v>-0.029033340361915</v>
       </c>
       <c r="U221" t="n">
-        <v>-0.0224071246882031</v>
+        <v>-0.0224273086066712</v>
       </c>
       <c r="V221" t="n">
-        <v>-0.025766078068649</v>
+        <v>-0.0257798956173732</v>
       </c>
       <c r="W221" t="n">
-        <v>-0.0298255615992624</v>
+        <v>-0.0298484109577703</v>
       </c>
       <c r="X221" t="n">
-        <v>-0.000453943809704966</v>
+        <v>-0.00048010593684826</v>
       </c>
       <c r="Y221" t="n">
-        <v>0.0132469502250108</v>
+        <v>0.0198615389538362</v>
       </c>
       <c r="Z221" t="n">
-        <v>0.18108667117246</v>
+        <v>0.182540185482219</v>
       </c>
       <c r="AA221" t="n">
-        <v>-0.0159127514453459</v>
+        <v>-0.0159290370424757</v>
       </c>
       <c r="AB221" t="n">
-        <v>-0.0780522336809329</v>
+        <v>-0.0781321147270974</v>
       </c>
       <c r="AC221" t="n">
-        <v>0.258358484194349</v>
+        <v>0.250791580396264</v>
       </c>
       <c r="AD221" t="n">
-        <v>0.0481820775385372</v>
+        <v>0.0661310911025787</v>
       </c>
       <c r="AE221" t="n">
-        <v>0.306540561732886</v>
+        <v>0.316922671498843</v>
       </c>
       <c r="AF221" t="n">
-        <v>0.212575576606607</v>
+        <v>0.22286151972927</v>
       </c>
       <c r="AG221" t="n">
-        <v>-0.0925533336591953</v>
+        <v>-0.0209359092488484</v>
       </c>
     </row>
     <row r="222">
@@ -23485,100 +23485,100 @@
         <v>255</v>
       </c>
       <c r="B222" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C222" t="n">
         <v>0</v>
       </c>
       <c r="D222" t="n">
-        <v>0.0242745484751063</v>
+        <v>0.024299391791382</v>
       </c>
       <c r="E222" t="n">
-        <v>-0.295596513481577</v>
+        <v>-0.295899036005608</v>
       </c>
       <c r="F222" t="n">
-        <v>-0.0121522534601843</v>
+        <v>-0.0121646904485173</v>
       </c>
       <c r="G222" t="n">
-        <v>-0.10806644570606</v>
+        <v>-0.108177044215945</v>
       </c>
       <c r="H222" t="n">
-        <v>-0.109022120647343</v>
+        <v>-0.113970594719517</v>
       </c>
       <c r="I222" t="n">
-        <v>0.0437047774083243</v>
+        <v>0.0412140954028463</v>
       </c>
       <c r="J222" t="n">
-        <v>-0.0458623242378591</v>
+        <v>-0.0461875757864698</v>
       </c>
       <c r="K222" t="n">
-        <v>0.0296643808796034</v>
+        <v>0.0296947403154162</v>
       </c>
       <c r="L222" t="n">
-        <v>0.0146317397304969</v>
+        <v>0.0145430056058064</v>
       </c>
       <c r="M222" t="n">
-        <v>-0.0355576564240909</v>
+        <v>-0.0271220291706298</v>
       </c>
       <c r="N222" t="n">
-        <v>0.0703338568877382</v>
+        <v>0.0717798750106577</v>
       </c>
       <c r="O222" t="n">
         <v>0</v>
       </c>
       <c r="P222" t="n">
-        <v>-0.096880277565739</v>
+        <v>-0.0969794278085916</v>
       </c>
       <c r="Q222" t="n">
-        <v>-0.0000480843054571453</v>
+        <v>0</v>
       </c>
       <c r="R222" t="n">
-        <v>-0.00312908399280576</v>
+        <v>-0.00311777151683929</v>
       </c>
       <c r="S222" t="n">
-        <v>-0.0600760350330372</v>
+        <v>-0.0601197879653204</v>
       </c>
       <c r="T222" t="n">
-        <v>-0.0281018740369811</v>
+        <v>-0.0281302074080254</v>
       </c>
       <c r="U222" t="n">
-        <v>-0.0152407652346435</v>
+        <v>-0.0152550024988492</v>
       </c>
       <c r="V222" t="n">
-        <v>-0.0103150884246051</v>
+        <v>-0.0103139931528964</v>
       </c>
       <c r="W222" t="n">
-        <v>-0.0295429020796404</v>
+        <v>-0.0295660125777588</v>
       </c>
       <c r="X222" t="n">
-        <v>-0.000654613094203388</v>
+        <v>-0.000680524807471519</v>
       </c>
       <c r="Y222" t="n">
-        <v>0.0397542452811134</v>
+        <v>0.0463310723073205</v>
       </c>
       <c r="Z222" t="n">
-        <v>0.0234671609856324</v>
+        <v>0.0247468960335807</v>
       </c>
       <c r="AA222" t="n">
-        <v>-0.283474218466655</v>
+        <v>-0.283764334662744</v>
       </c>
       <c r="AB222" t="n">
-        <v>0.199682321235701</v>
+        <v>0.199886682238181</v>
       </c>
       <c r="AC222" t="n">
-        <v>-0.0668835468667779</v>
+        <v>-0.0747063291819175</v>
       </c>
       <c r="AD222" t="n">
-        <v>-0.14599111703672</v>
+        <v>-0.128426913554824</v>
       </c>
       <c r="AE222" t="n">
-        <v>-0.212874663903498</v>
+        <v>-0.203133242736741</v>
       </c>
       <c r="AF222" t="n">
-        <v>-0.296666561134451</v>
+        <v>-0.287010895161304</v>
       </c>
       <c r="AG222" t="n">
-        <v>-0.174026140163818</v>
+        <v>-0.0999947992601838</v>
       </c>
     </row>
     <row r="223">
@@ -23586,100 +23586,100 @@
         <v>256</v>
       </c>
       <c r="B223" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C223" t="n">
         <v>0</v>
       </c>
       <c r="D223" t="n">
-        <v>0.0365371038719133</v>
+        <v>0.0365744970629018</v>
       </c>
       <c r="E223" t="n">
-        <v>-0.125137317980377</v>
+        <v>-0.125265387343713</v>
       </c>
       <c r="F223" t="n">
-        <v>-0.0670668327775431</v>
+        <v>-0.067135471028014</v>
       </c>
       <c r="G223" t="n">
-        <v>-0.106551395513561</v>
+        <v>-0.106660443474682</v>
       </c>
       <c r="H223" t="n">
-        <v>-0.104655154659296</v>
+        <v>-0.109550048486844</v>
       </c>
       <c r="I223" t="n">
-        <v>-0.026033241121188</v>
+        <v>-0.0285695521087803</v>
       </c>
       <c r="J223" t="n">
-        <v>-0.0242599754784635</v>
+        <v>-0.0245602926817725</v>
       </c>
       <c r="K223" t="n">
-        <v>0.0285096032945109</v>
+        <v>0.02853878089558</v>
       </c>
       <c r="L223" t="n">
-        <v>-0.00563051329825817</v>
+        <v>-0.00573893143726738</v>
       </c>
       <c r="M223" t="n">
-        <v>-0.0753813095968302</v>
+        <v>-0.0754584571374945</v>
       </c>
       <c r="N223" t="n">
-        <v>0.0144845669768829</v>
+        <v>0.0737299342243676</v>
       </c>
       <c r="O223" t="n">
         <v>0</v>
       </c>
       <c r="P223" t="n">
-        <v>-0.094073687775945</v>
+        <v>-0.0941699656688597</v>
       </c>
       <c r="Q223" t="n">
-        <v>-0.000250159180265797</v>
+        <v>0</v>
       </c>
       <c r="R223" t="n">
-        <v>-0.00283618246089614</v>
+        <v>-0.00305229291859512</v>
       </c>
       <c r="S223" t="n">
-        <v>-0.0947096501618208</v>
+        <v>-0.0948380956054129</v>
       </c>
       <c r="T223" t="n">
-        <v>-0.0265263478885997</v>
+        <v>-0.0265530731529042</v>
       </c>
       <c r="U223" t="n">
-        <v>-0.0138302049317022</v>
+        <v>-0.0138430124000316</v>
       </c>
       <c r="V223" t="n">
-        <v>-0.00983952557423932</v>
+        <v>-0.00984267540133323</v>
       </c>
       <c r="W223" t="n">
-        <v>-0.0233250353506812</v>
+        <v>-0.0233446755420331</v>
       </c>
       <c r="X223" t="n">
-        <v>-0.00133717229597802</v>
+        <v>-0.00138469069866384</v>
       </c>
       <c r="Y223" t="n">
-        <v>0.012843116489513</v>
+        <v>0.0128562605282267</v>
       </c>
       <c r="Z223" t="n">
-        <v>-0.0207758018101161</v>
+        <v>-0.0207970644019117</v>
       </c>
       <c r="AA223" t="n">
-        <v>-0.155667046886007</v>
+        <v>-0.155826361308825</v>
       </c>
       <c r="AB223" t="n">
-        <v>0.0856527552443594</v>
+        <v>0.0857404148970448</v>
       </c>
       <c r="AC223" t="n">
-        <v>-0.132069281262695</v>
+        <v>-0.139880043819084</v>
       </c>
       <c r="AD223" t="n">
-        <v>-0.335557393560679</v>
+        <v>-0.276697808174646</v>
       </c>
       <c r="AE223" t="n">
-        <v>-0.467626674823374</v>
+        <v>-0.41657785199373</v>
       </c>
       <c r="AF223" t="n">
-        <v>-0.537640966465021</v>
+        <v>-0.48666379840551</v>
       </c>
       <c r="AG223" t="n">
-        <v>-0.228212703969084</v>
+        <v>-0.209925093491481</v>
       </c>
     </row>
     <row r="224">
@@ -23687,100 +23687,100 @@
         <v>257</v>
       </c>
       <c r="B224" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C224" t="n">
         <v>0</v>
       </c>
       <c r="D224" t="n">
-        <v>0.0415369779028945</v>
+        <v>0.0415794881180789</v>
       </c>
       <c r="E224" t="n">
-        <v>-0.0262771765184012</v>
+        <v>-0.0263040693855434</v>
       </c>
       <c r="F224" t="n">
-        <v>-0.0111532785660524</v>
+        <v>-0.0111646931728869</v>
       </c>
       <c r="G224" t="n">
-        <v>-0.120013563055343</v>
+        <v>-0.120136388610983</v>
       </c>
       <c r="H224" t="n">
-        <v>-0.0682861450211372</v>
+        <v>-0.0730945354248257</v>
       </c>
       <c r="I224" t="n">
-        <v>0.00569971835599107</v>
+        <v>0.00322171668885812</v>
       </c>
       <c r="J224" t="n">
-        <v>-0.0313923451803699</v>
+        <v>-0.0316971261721691</v>
       </c>
       <c r="K224" t="n">
-        <v>0.0273675737717791</v>
+        <v>0.027395582584862</v>
       </c>
       <c r="L224" t="n">
-        <v>-0.00505034872202343</v>
+        <v>-0.00515711643387423</v>
       </c>
       <c r="M224" t="n">
-        <v>-0.0748325683720228</v>
+        <v>-0.0749091543141134</v>
       </c>
       <c r="N224" t="n">
-        <v>0.0147498395713569</v>
+        <v>0.0147649350088627</v>
       </c>
       <c r="O224" t="n">
         <v>0</v>
       </c>
       <c r="P224" t="n">
-        <v>-0.00101858021815379</v>
+        <v>-0.00101962266434132</v>
       </c>
       <c r="Q224" t="n">
-        <v>-0.0001646233892468</v>
+        <v>0</v>
       </c>
       <c r="R224" t="n">
-        <v>-0.00218707785682872</v>
+        <v>-0.00233365005398452</v>
       </c>
       <c r="S224" t="n">
-        <v>-0.0708071718458687</v>
+        <v>-0.0708275862149756</v>
       </c>
       <c r="T224" t="n">
-        <v>-0.0258328785956326</v>
+        <v>-0.0258588984923155</v>
       </c>
       <c r="U224" t="n">
-        <v>-0.0139537190435213</v>
+        <v>-0.0139666667828971</v>
       </c>
       <c r="V224" t="n">
-        <v>-0.00834123712353133</v>
+        <v>-0.00834596879418591</v>
       </c>
       <c r="W224" t="n">
-        <v>0.000189201448040142</v>
+        <v>0.000191721643312038</v>
       </c>
       <c r="X224" t="n">
-        <v>-0.000348427611235486</v>
+        <v>-0.000351769766428433</v>
       </c>
       <c r="Y224" t="n">
-        <v>-0.0202353726958458</v>
+        <v>-0.0202560821959362</v>
       </c>
       <c r="Z224" t="n">
-        <v>-0.0238346810708362</v>
+        <v>-0.0238590742133402</v>
       </c>
       <c r="AA224" t="n">
-        <v>0.00410652281844098</v>
+        <v>0.00411072555964858</v>
       </c>
       <c r="AB224" t="n">
-        <v>-0.0825831079708898</v>
+        <v>-0.0826676260525528</v>
       </c>
       <c r="AC224" t="n">
-        <v>-0.0716615467957604</v>
+        <v>-0.0793314787571489</v>
       </c>
       <c r="AD224" t="n">
-        <v>-0.226617296803327</v>
+        <v>-0.226771816840343</v>
       </c>
       <c r="AE224" t="n">
-        <v>-0.298278843599087</v>
+        <v>-0.306103295597492</v>
       </c>
       <c r="AF224" t="n">
-        <v>-0.376755428751536</v>
+        <v>-0.384660196090397</v>
       </c>
       <c r="AG224" t="n">
-        <v>-0.249621844936101</v>
+        <v>-0.233868342481987</v>
       </c>
     </row>
     <row r="225">
@@ -23788,100 +23788,100 @@
         <v>258</v>
       </c>
       <c r="B225" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C225" t="n">
         <v>0</v>
       </c>
       <c r="D225" t="n">
-        <v>-0.0920039215058041</v>
+        <v>-0.0920980811365349</v>
       </c>
       <c r="E225" t="n">
-        <v>-0.0773638393681652</v>
+        <v>-0.0774430158905091</v>
       </c>
       <c r="F225" t="n">
-        <v>-0.0110028907801561</v>
+        <v>-0.0110141514755251</v>
       </c>
       <c r="G225" t="n">
-        <v>-0.121391774732743</v>
+        <v>-0.121516010792419</v>
       </c>
       <c r="H225" t="n">
-        <v>-0.0740754703813422</v>
+        <v>-0.0788424406145329</v>
       </c>
       <c r="I225" t="n">
-        <v>0.0191478114252186</v>
+        <v>0.016708390383198</v>
       </c>
       <c r="J225" t="n">
-        <v>-0.0403150626449094</v>
+        <v>-0.0406262511837659</v>
       </c>
       <c r="K225" t="n">
-        <v>0.0264575553293169</v>
+        <v>0.026484632801658</v>
       </c>
       <c r="L225" t="n">
-        <v>0.00112002694786687</v>
+        <v>0.00102058932224835</v>
       </c>
       <c r="M225" t="n">
-        <v>-0.129174934233444</v>
+        <v>-0.129307135816899</v>
       </c>
       <c r="N225" t="n">
-        <v>0.0148405618576446</v>
+        <v>0.0148557501431164</v>
       </c>
       <c r="O225" t="n">
         <v>0</v>
       </c>
       <c r="P225" t="n">
-        <v>-0.000986093993669235</v>
+        <v>-0.000987103192459789</v>
       </c>
       <c r="Q225" t="n">
-        <v>-0.00000214213223808329</v>
+        <v>0</v>
       </c>
       <c r="R225" t="n">
-        <v>-0.00306670370175271</v>
+        <v>-0.00305173299732271</v>
       </c>
       <c r="S225" t="n">
-        <v>-0.0326678805608594</v>
+        <v>-0.0326497820916149</v>
       </c>
       <c r="T225" t="n">
-        <v>-0.00387080743876697</v>
+        <v>-0.00387435485837908</v>
       </c>
       <c r="U225" t="n">
-        <v>-0.0130106371267025</v>
+        <v>-0.0130226330051808</v>
       </c>
       <c r="V225" t="n">
-        <v>-0.00757316523605586</v>
+        <v>-0.00757714885644937</v>
       </c>
       <c r="W225" t="n">
-        <v>0.000131513369542487</v>
+        <v>0.000133951279051296</v>
       </c>
       <c r="X225" t="n">
-        <v>-0.000340010066034549</v>
+        <v>-0.00034331377595608</v>
       </c>
       <c r="Y225" t="n">
-        <v>-0.00626637013995236</v>
+        <v>-0.00627278333505039</v>
       </c>
       <c r="Z225" t="n">
-        <v>-0.021653053680598</v>
+        <v>-0.0216752140788222</v>
       </c>
       <c r="AA225" t="n">
-        <v>-0.180370651654125</v>
+        <v>-0.180555248502569</v>
       </c>
       <c r="AB225" t="n">
-        <v>-0.0330250445844222</v>
+        <v>-0.0330588434263851</v>
       </c>
       <c r="AC225" t="n">
-        <v>-0.0676651393238492</v>
+        <v>-0.0752550792911945</v>
       </c>
       <c r="AD225" t="n">
-        <v>-0.203639723082887</v>
+        <v>-0.203771500585966</v>
       </c>
       <c r="AE225" t="n">
-        <v>-0.271304862406736</v>
+        <v>-0.279026579877161</v>
       </c>
       <c r="AF225" t="n">
-        <v>-0.484700558645283</v>
+        <v>-0.492640671806115</v>
       </c>
       <c r="AG225" t="n">
-        <v>-0.423940878749074</v>
+        <v>-0.412743890365833</v>
       </c>
     </row>
     <row r="226">
@@ -23889,100 +23889,100 @@
         <v>259</v>
       </c>
       <c r="B226" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C226" t="n">
         <v>0</v>
       </c>
       <c r="D226" t="n">
-        <v>-0.0746106608664148</v>
+        <v>-0.0746870197015686</v>
       </c>
       <c r="E226" t="n">
-        <v>-0.0233506572251125</v>
+        <v>-0.0233745550027904</v>
       </c>
       <c r="F226" t="n">
-        <v>-0.0108875432753289</v>
+        <v>-0.0108986859205292</v>
       </c>
       <c r="G226" t="n">
-        <v>-0.108856827426225</v>
+        <v>-0.108968234836966</v>
       </c>
       <c r="H226" t="n">
-        <v>-0.0259014770375749</v>
+        <v>-0.0305750850946892</v>
       </c>
       <c r="I226" t="n">
-        <v>0.0031910303152314</v>
+        <v>0.000758373743556107</v>
       </c>
       <c r="J226" t="n">
-        <v>-0.0381445448756897</v>
+        <v>-0.0384509768642541</v>
       </c>
       <c r="K226" t="n">
-        <v>0.00933741731862908</v>
+        <v>0.00934697351745531</v>
       </c>
       <c r="L226" t="n">
-        <v>0.00644659175199075</v>
+        <v>0.00635355018134651</v>
       </c>
       <c r="M226" t="n">
-        <v>-0.119939656098652</v>
+        <v>-0.120062406015649</v>
       </c>
       <c r="N226" t="n">
-        <v>0.0152430734684407</v>
+        <v>0.0152586736966212</v>
       </c>
       <c r="O226" t="n">
         <v>0</v>
       </c>
       <c r="P226" t="n">
-        <v>-0.000954733111722777</v>
+        <v>-0.000955710214826373</v>
       </c>
       <c r="Q226" t="n">
-        <v>-0.0000415290684768083</v>
+        <v>0</v>
       </c>
       <c r="R226" t="n">
-        <v>-0.00295067625147927</v>
+        <v>-0.00297921694212841</v>
       </c>
       <c r="S226" t="n">
-        <v>-0.0136404889667323</v>
+        <v>-0.0136034012694774</v>
       </c>
       <c r="T226" t="n">
-        <v>-0.00265250503418386</v>
+        <v>-0.0026548094948828</v>
       </c>
       <c r="U226" t="n">
-        <v>-0.0144094884045077</v>
+        <v>-0.0144229283039801</v>
       </c>
       <c r="V226" t="n">
-        <v>-0.0069924643383737</v>
+        <v>-0.00699663535314229</v>
       </c>
       <c r="W226" t="n">
-        <v>-0.00014888998171876</v>
+        <v>-0.000147217014738937</v>
       </c>
       <c r="X226" t="n">
-        <v>-0.000331480211150204</v>
+        <v>-0.000334747431066952</v>
       </c>
       <c r="Y226" t="n">
-        <v>0.0100108888418354</v>
+        <v>0.0100211342920424</v>
       </c>
       <c r="Z226" t="n">
-        <v>-0.0190541484795073</v>
+        <v>-0.0190736490785617</v>
       </c>
       <c r="AA226" t="n">
-        <v>-0.108848861366856</v>
+        <v>-0.108960260624888</v>
       </c>
       <c r="AB226" t="n">
-        <v>-0.0746186269257839</v>
+        <v>-0.0746949939136468</v>
       </c>
       <c r="AC226" t="n">
-        <v>-0.0450709825274134</v>
+        <v>-0.0525671645165854</v>
       </c>
       <c r="AD226" t="n">
-        <v>-0.155862097636228</v>
+        <v>-0.15595091312979</v>
       </c>
       <c r="AE226" t="n">
-        <v>-0.200933080163642</v>
+        <v>-0.208518077646376</v>
       </c>
       <c r="AF226" t="n">
-        <v>-0.384400568456282</v>
+        <v>-0.392173332184911</v>
       </c>
       <c r="AG226" t="n">
-        <v>-0.445874380579532</v>
+        <v>-0.439034499621734</v>
       </c>
     </row>
     <row r="227">
@@ -23990,43 +23990,43 @@
         <v>260</v>
       </c>
       <c r="B227" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C227" t="n">
         <v>0</v>
       </c>
       <c r="D227" t="n">
-        <v>-25.8756663615161</v>
+        <v>-25.9021483108683</v>
       </c>
       <c r="E227" t="n">
-        <v>-5.5750845144171</v>
+        <v>-5.58079022663653</v>
       </c>
       <c r="F227" t="n">
-        <v>-0.984822718777161</v>
+        <v>-0.985830616506059</v>
       </c>
       <c r="G227" t="n">
-        <v>-43.6424551793561</v>
+        <v>-43.6871202044618</v>
       </c>
       <c r="H227" t="n">
-        <v>7.4864500322914</v>
+        <v>7.4941118945141</v>
       </c>
       <c r="I227" t="n">
-        <v>3.94052739620026</v>
+        <v>3.9445602526094</v>
       </c>
       <c r="J227" t="n">
-        <v>0.200916845261599</v>
+        <v>0.200857393265418</v>
       </c>
       <c r="K227" t="n">
-        <v>-1.98438910578723</v>
+        <v>-1.98641999036659</v>
       </c>
       <c r="L227" t="n">
-        <v>0.0747950734417034</v>
+        <v>0.0747728452778162</v>
       </c>
       <c r="M227" t="n">
-        <v>-6.48234448022495</v>
+        <v>-6.48897871007666</v>
       </c>
       <c r="N227" t="n">
-        <v>-0.647165271367948</v>
+        <v>-0.647827600124989</v>
       </c>
       <c r="O227" t="n">
         <v>0</v>
@@ -24035,55 +24035,55 @@
         <v>0</v>
       </c>
       <c r="Q227" t="n">
-        <v>-0.00015794510706083</v>
+        <v>0</v>
       </c>
       <c r="R227" t="n">
-        <v>-0.0610809492404758</v>
+        <v>-0.0613015681073477</v>
       </c>
       <c r="S227" t="n">
-        <v>-0.0723925109326546</v>
+        <v>-0.0725475116591895</v>
       </c>
       <c r="T227" t="n">
-        <v>-0.00222671263613884</v>
+        <v>-0.00222858488261831</v>
       </c>
       <c r="U227" t="n">
-        <v>-0.00987366777659905</v>
+        <v>-0.00988247690669468</v>
       </c>
       <c r="V227" t="n">
-        <v>-0.00641949186203841</v>
+        <v>-0.00642606176659591</v>
       </c>
       <c r="W227" t="n">
-        <v>-0.00722401508045198</v>
+        <v>-0.00723140835870835</v>
       </c>
       <c r="X227" t="n">
-        <v>-0.00026258398263994</v>
+        <v>-0.000327429332277272</v>
       </c>
       <c r="Y227" t="n">
-        <v>-5.10381257273806</v>
+        <v>-5.10903597082048</v>
       </c>
       <c r="Z227" t="n">
-        <v>-0.991920629870226</v>
+        <v>-0.992935791818698</v>
       </c>
       <c r="AA227" t="n">
-        <v>-32.4355735947104</v>
+        <v>-32.4687691540109</v>
       </c>
       <c r="AB227" t="n">
-        <v>-37.0825479461619</v>
+        <v>-37.1204993613192</v>
       </c>
       <c r="AC227" t="n">
-        <v>9.71830024140774</v>
+        <v>9.72788239530015</v>
       </c>
       <c r="AD227" t="n">
-        <v>-13.3848808308192</v>
+        <v>-13.3987231138543</v>
       </c>
       <c r="AE227" t="n">
-        <v>-3.66658058941151</v>
+        <v>-3.67084071855412</v>
       </c>
       <c r="AF227" t="n">
-        <v>-73.1847021302838</v>
+        <v>-73.2601092338842</v>
       </c>
       <c r="AG227" t="n">
-        <v>-18.6076396715342</v>
+        <v>-18.6323958584914</v>
       </c>
     </row>
     <row r="228">
@@ -24091,7 +24091,7 @@
         <v>261</v>
       </c>
       <c r="B228" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C228" t="n">
         <v>0</v>
@@ -24109,25 +24109,25 @@
         <v>0</v>
       </c>
       <c r="H228" t="n">
-        <v>7.4495150214336</v>
+        <v>7.45713908323512</v>
       </c>
       <c r="I228" t="n">
-        <v>3.91215399671427</v>
+        <v>3.91615781491749</v>
       </c>
       <c r="J228" t="n">
-        <v>0.203510104418812</v>
+        <v>0.203455616097685</v>
       </c>
       <c r="K228" t="n">
         <v>0</v>
       </c>
       <c r="L228" t="n">
-        <v>0.0725424916255429</v>
+        <v>0.0725188187494703</v>
       </c>
       <c r="M228" t="n">
-        <v>-6.38101689279858</v>
+        <v>-6.38754742089434</v>
       </c>
       <c r="N228" t="n">
-        <v>-0.645209655620347</v>
+        <v>-0.645869982940344</v>
       </c>
       <c r="O228" t="n">
         <v>0</v>
@@ -24139,31 +24139,31 @@
         <v>0</v>
       </c>
       <c r="R228" t="n">
-        <v>-0.0512677812081671</v>
+        <v>-0.0513202502254431</v>
       </c>
       <c r="S228" t="n">
-        <v>-0.0620237414912851</v>
+        <v>-0.0620470869069511</v>
       </c>
       <c r="T228" t="n">
-        <v>-0.00282028254093768</v>
+        <v>-0.00282276580815021</v>
       </c>
       <c r="U228" t="n">
-        <v>-0.00673398576398523</v>
+        <v>-0.0067401067756584</v>
       </c>
       <c r="V228" t="n">
-        <v>-0.00575331375598581</v>
+        <v>-0.00575920187346902</v>
       </c>
       <c r="W228" t="n">
-        <v>-0.00609005423527493</v>
+        <v>-0.00609628698327674</v>
       </c>
       <c r="X228" t="n">
-        <v>-0.000257083888041818</v>
+        <v>-0.000259648842097867</v>
       </c>
       <c r="Y228" t="n">
-        <v>-5.05484246450805</v>
+        <v>-5.06001574508208</v>
       </c>
       <c r="Z228" t="n">
-        <v>-0.977560933496748</v>
+        <v>-0.97856139929221</v>
       </c>
       <c r="AA228" t="n">
         <v>0</v>
@@ -24172,19 +24172,19 @@
         <v>0</v>
       </c>
       <c r="AC228" t="n">
-        <v>11.6377216141922</v>
+        <v>11.6492713329998</v>
       </c>
       <c r="AD228" t="n">
-        <v>-13.1935761893074</v>
+        <v>-13.207039895624</v>
       </c>
       <c r="AE228" t="n">
-        <v>-1.55585457511517</v>
+        <v>-1.55776856262425</v>
       </c>
       <c r="AF228" t="n">
-        <v>-1.55585457511517</v>
+        <v>-1.55776856262425</v>
       </c>
       <c r="AG228" t="n">
-        <v>-18.9024144581251</v>
+        <v>-18.9256729501249</v>
       </c>
     </row>
     <row r="229">
@@ -24192,7 +24192,7 @@
         <v>262</v>
       </c>
       <c r="B229" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C229" t="n">
         <v>0</v>
@@ -24210,25 +24210,25 @@
         <v>0</v>
       </c>
       <c r="H229" t="n">
-        <v>3.6884966724691</v>
+        <v>3.69227159291757</v>
       </c>
       <c r="I229" t="n">
-        <v>1.94244400486308</v>
+        <v>1.94443196154167</v>
       </c>
       <c r="J229" t="n">
-        <v>0.204845412073885</v>
+        <v>0.204794652573815</v>
       </c>
       <c r="K229" t="n">
         <v>0</v>
       </c>
       <c r="L229" t="n">
-        <v>0.0785359114100979</v>
+        <v>0.078519252622395</v>
       </c>
       <c r="M229" t="n">
-        <v>-6.23307845165189</v>
+        <v>-6.23945757501661</v>
       </c>
       <c r="N229" t="n">
-        <v>-0.643202146827087</v>
+        <v>-0.643860419601109</v>
       </c>
       <c r="O229" t="n">
         <v>0</v>
@@ -24240,31 +24240,31 @@
         <v>0</v>
       </c>
       <c r="R229" t="n">
-        <v>-0.0474346821227481</v>
+        <v>-0.0474832282290381</v>
       </c>
       <c r="S229" t="n">
-        <v>-0.0571594585636327</v>
+        <v>-0.0571781864988972</v>
       </c>
       <c r="T229" t="n">
-        <v>-0.000297915771048229</v>
+        <v>-0.000297821194628747</v>
       </c>
       <c r="U229" t="n">
-        <v>-0.00306504171538251</v>
+        <v>-0.0030674147463155</v>
       </c>
       <c r="V229" t="n">
-        <v>-0.00318998736084214</v>
+        <v>-0.0031932520915951</v>
       </c>
       <c r="W229" t="n">
-        <v>-0.0056712417580123</v>
+        <v>-0.00567704588049948</v>
       </c>
       <c r="X229" t="n">
-        <v>-0.000252004453182972</v>
+        <v>-0.000254543515602714</v>
       </c>
       <c r="Y229" t="n">
-        <v>-5.01882654391291</v>
+        <v>-5.02396296469088</v>
       </c>
       <c r="Z229" t="n">
-        <v>-0.965195836511259</v>
+        <v>-0.966183647487806</v>
       </c>
       <c r="AA229" t="n">
         <v>0</v>
@@ -24273,19 +24273,19 @@
         <v>0</v>
       </c>
       <c r="AC229" t="n">
-        <v>5.91432200081617</v>
+        <v>5.92001745965545</v>
       </c>
       <c r="AD229" t="n">
-        <v>-12.977373310648</v>
+        <v>-12.990616098953</v>
       </c>
       <c r="AE229" t="n">
-        <v>-7.06305130983182</v>
+        <v>-7.07059863929753</v>
       </c>
       <c r="AF229" t="n">
-        <v>-7.06305130983182</v>
+        <v>-7.07059863929753</v>
       </c>
       <c r="AG229" t="n">
-        <v>-20.5470021459218</v>
+        <v>-20.5701624419977</v>
       </c>
     </row>
     <row r="230">
@@ -24293,7 +24293,7 @@
         <v>263</v>
       </c>
       <c r="B230" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C230" t="n">
         <v>0</v>
@@ -24311,25 +24311,25 @@
         <v>0</v>
       </c>
       <c r="H230" t="n">
-        <v>3.67438275212426</v>
+        <v>3.67814322795443</v>
       </c>
       <c r="I230" t="n">
-        <v>1.92423486421429</v>
+        <v>1.92620418510071</v>
       </c>
       <c r="J230" t="n">
-        <v>0.210861216229905</v>
+        <v>0.210818958159114</v>
       </c>
       <c r="K230" t="n">
         <v>0</v>
       </c>
       <c r="L230" t="n">
-        <v>0.0783198919017364</v>
+        <v>0.0783038857304531</v>
       </c>
       <c r="M230" t="n">
-        <v>-6.23999255253099</v>
+        <v>-6.24637875199829</v>
       </c>
       <c r="N230" t="n">
-        <v>-0.641300618413374</v>
+        <v>-0.641956945104986</v>
       </c>
       <c r="O230" t="n">
         <v>0</v>
@@ -24341,31 +24341,31 @@
         <v>0</v>
       </c>
       <c r="R230" t="n">
-        <v>-0.043694143254606</v>
+        <v>-0.0437388611788707</v>
       </c>
       <c r="S230" t="n">
-        <v>-0.0515863813622249</v>
+        <v>-0.0515997637341654</v>
       </c>
       <c r="T230" t="n">
-        <v>-0.000291260502732673</v>
+        <v>-0.000291162711940699</v>
       </c>
       <c r="U230" t="n">
-        <v>-0.00136497824116449</v>
+        <v>-0.00136561825253717</v>
       </c>
       <c r="V230" t="n">
-        <v>-0.0018018637802496</v>
+        <v>-0.00180370786282129</v>
       </c>
       <c r="W230" t="n">
-        <v>-0.00523385223062858</v>
+        <v>-0.00523920871527912</v>
       </c>
       <c r="X230" t="n">
-        <v>-0.000246353835379716</v>
+        <v>-0.000248866575381462</v>
       </c>
       <c r="Y230" t="n">
-        <v>-4.98373051975877</v>
+        <v>-4.98883102219087</v>
       </c>
       <c r="Z230" t="n">
-        <v>-0.953041348816851</v>
+        <v>-0.954016720518482</v>
       </c>
       <c r="AA230" t="n">
         <v>0</v>
@@ -24374,19 +24374,19 @@
         <v>0</v>
       </c>
       <c r="AC230" t="n">
-        <v>5.88779872447019</v>
+        <v>5.89347025694471</v>
       </c>
       <c r="AD230" t="n">
-        <v>-12.922283872727</v>
+        <v>-12.9354706288436</v>
       </c>
       <c r="AE230" t="n">
-        <v>-7.03448514825678</v>
+        <v>-7.04200037189891</v>
       </c>
       <c r="AF230" t="n">
-        <v>-7.03448514825678</v>
+        <v>-7.04200037189891</v>
       </c>
       <c r="AG230" t="n">
-        <v>-22.2095232908719</v>
+        <v>-22.2326192019262</v>
       </c>
     </row>
     <row r="231">
@@ -24394,7 +24394,7 @@
         <v>264</v>
       </c>
       <c r="B231" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C231" t="n">
         <v>0</v>
@@ -24412,19 +24412,19 @@
         <v>0</v>
       </c>
       <c r="H231" t="n">
-        <v>3.62885834870484</v>
+        <v>3.63257223346645</v>
       </c>
       <c r="I231" t="n">
-        <v>1.90642107030752</v>
+        <v>1.90837216001174</v>
       </c>
       <c r="J231" t="n">
-        <v>0.211218791166407</v>
+        <v>0.211434958945499</v>
       </c>
       <c r="K231" t="n">
         <v>0</v>
       </c>
       <c r="L231" t="n">
-        <v>0.0782565982265536</v>
+        <v>0.0783366884256524</v>
       </c>
       <c r="M231" t="n">
         <v>0</v>
@@ -24442,25 +24442,25 @@
         <v>0</v>
       </c>
       <c r="R231" t="n">
-        <v>-0.0259900494802466</v>
+        <v>-0.0260166484927853</v>
       </c>
       <c r="S231" t="n">
-        <v>-0.0434268499974092</v>
+        <v>-0.0437706549060446</v>
       </c>
       <c r="T231" t="n">
-        <v>-0.000284912122655975</v>
+        <v>-0.000285203710447245</v>
       </c>
       <c r="U231" t="n">
-        <v>-0.0010332813506301</v>
+        <v>-0.001033713599852</v>
       </c>
       <c r="V231" t="n">
-        <v>-0.00152135873278938</v>
+        <v>-0.00152291573790551</v>
       </c>
       <c r="W231" t="n">
-        <v>-0.00311147577184435</v>
+        <v>-0.00311466015143285</v>
       </c>
       <c r="X231" t="n">
-        <v>-0.000082917942610205</v>
+        <v>-0.000243945894346533</v>
       </c>
       <c r="Y231" t="n">
         <v>0</v>
@@ -24475,19 +24475,19 @@
         <v>0</v>
       </c>
       <c r="AC231" t="n">
-        <v>5.82475480840532</v>
+        <v>5.83071604084934</v>
       </c>
       <c r="AD231" t="n">
-        <v>-0.0754508453981859</v>
+        <v>-0.075987742492814</v>
       </c>
       <c r="AE231" t="n">
-        <v>5.74930396300713</v>
+        <v>5.75472829835652</v>
       </c>
       <c r="AF231" t="n">
-        <v>5.74930396300713</v>
+        <v>5.75472829835652</v>
       </c>
       <c r="AG231" t="n">
-        <v>-2.47602176754916</v>
+        <v>-2.47890981886604</v>
       </c>
     </row>
     <row r="232">
@@ -24495,7 +24495,7 @@
         <v>265</v>
       </c>
       <c r="B232" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C232" t="n">
         <v>0</v>
@@ -24513,19 +24513,19 @@
         <v>0</v>
       </c>
       <c r="H232" t="n">
-        <v>3.58500749025487</v>
+        <v>3.58867649670509</v>
       </c>
       <c r="I232" t="n">
-        <v>1.88850323451037</v>
+        <v>1.89043598655273</v>
       </c>
       <c r="J232" t="n">
-        <v>0.212069129670361</v>
+        <v>0.212286167711918</v>
       </c>
       <c r="K232" t="n">
         <v>0</v>
       </c>
       <c r="L232" t="n">
-        <v>0.0779285144465309</v>
+        <v>0.0780082688746421</v>
       </c>
       <c r="M232" t="n">
         <v>0</v>
@@ -24543,25 +24543,25 @@
         <v>0</v>
       </c>
       <c r="R232" t="n">
-        <v>-0.014348116367449</v>
+        <v>-0.0143628006691258</v>
       </c>
       <c r="S232" t="n">
-        <v>-0.0430621427476047</v>
+        <v>-0.0430933043477204</v>
       </c>
       <c r="T232" t="n">
-        <v>-0.000279337598189915</v>
+        <v>-0.000279623480842136</v>
       </c>
       <c r="U232" t="n">
-        <v>-0.00101767945820255</v>
+        <v>-0.00101822510965699</v>
       </c>
       <c r="V232" t="n">
-        <v>-0.00125832627961714</v>
+        <v>-0.00125961408926578</v>
       </c>
       <c r="W232" t="n">
-        <v>-0.00172060770021725</v>
+        <v>-0.00172236862282831</v>
       </c>
       <c r="X232" t="n">
-        <v>-0.0000813056032428949</v>
+        <v>-0.0000821292712246784</v>
       </c>
       <c r="Y232" t="n">
         <v>0</v>
@@ -24576,19 +24576,19 @@
         <v>0</v>
       </c>
       <c r="AC232" t="n">
-        <v>5.76350836888213</v>
+        <v>5.76940691984437</v>
       </c>
       <c r="AD232" t="n">
-        <v>-0.0617675157545235</v>
+        <v>-0.0618180655906641</v>
       </c>
       <c r="AE232" t="n">
-        <v>5.70174085312761</v>
+        <v>5.70758885425371</v>
       </c>
       <c r="AF232" t="n">
-        <v>5.70174085312761</v>
+        <v>5.70758885425371</v>
       </c>
       <c r="AG232" t="n">
-        <v>-0.661622910488465</v>
+        <v>-0.66257046464655</v>
       </c>
     </row>
     <row r="233">
@@ -24596,7 +24596,7 @@
         <v>266</v>
       </c>
       <c r="B233" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C233" t="n">
         <v>0</v>
@@ -24614,19 +24614,19 @@
         <v>0</v>
       </c>
       <c r="H233" t="n">
-        <v>3.54194159359358</v>
+        <v>3.54556652508633</v>
       </c>
       <c r="I233" t="n">
-        <v>1.87053012085925</v>
+        <v>1.8724444786667</v>
       </c>
       <c r="J233" t="n">
-        <v>0.212143487434851</v>
+        <v>0.212360601576421</v>
       </c>
       <c r="K233" t="n">
         <v>0</v>
       </c>
       <c r="L233" t="n">
-        <v>0.0770512921203527</v>
+        <v>0.077130148772272</v>
       </c>
       <c r="M233" t="n">
         <v>0</v>
@@ -24644,25 +24644,25 @@
         <v>0</v>
       </c>
       <c r="R233" t="n">
-        <v>-0.0140803041868102</v>
+        <v>-0.0140947144013001</v>
       </c>
       <c r="S233" t="n">
-        <v>-0.0439655536457457</v>
+        <v>-0.0439977516982846</v>
       </c>
       <c r="T233" t="n">
-        <v>0.000201757887794612</v>
+        <v>0.000201964372995469</v>
       </c>
       <c r="U233" t="n">
-        <v>-0.00101167744077242</v>
+        <v>-0.00101234414072635</v>
       </c>
       <c r="V233" t="n">
-        <v>-0.000244521466260629</v>
+        <v>-0.000244771717017249</v>
       </c>
       <c r="W233" t="n">
-        <v>-0.00170061288176996</v>
+        <v>-0.00170235334107151</v>
       </c>
       <c r="X233" t="n">
-        <v>-0.0000798606087363539</v>
+        <v>-0.0000806763810526921</v>
       </c>
       <c r="Y233" t="n">
         <v>0</v>
@@ -24677,19 +24677,19 @@
         <v>0</v>
       </c>
       <c r="AC233" t="n">
-        <v>5.70166649400803</v>
+        <v>5.70750175410172</v>
       </c>
       <c r="AD233" t="n">
-        <v>-0.0608807723423007</v>
+        <v>-0.060930647306457</v>
       </c>
       <c r="AE233" t="n">
-        <v>5.64078572166573</v>
+        <v>5.64657110679527</v>
       </c>
       <c r="AF233" t="n">
-        <v>5.64078572166573</v>
+        <v>5.64657110679527</v>
       </c>
       <c r="AG233" t="n">
-        <v>2.51433634738592</v>
+        <v>2.51672197187665</v>
       </c>
     </row>
     <row r="234">
@@ -24697,7 +24697,7 @@
         <v>267</v>
       </c>
       <c r="B234" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C234" t="n">
         <v>0</v>
@@ -24715,19 +24715,19 @@
         <v>0</v>
       </c>
       <c r="H234" t="n">
-        <v>3.53674909321989</v>
+        <v>3.54036871054874</v>
       </c>
       <c r="I234" t="n">
-        <v>1.85087544179138</v>
+        <v>1.85276968439838</v>
       </c>
       <c r="J234" t="n">
-        <v>0.212155656068045</v>
+        <v>0.212372782663367</v>
       </c>
       <c r="K234" t="n">
         <v>0</v>
       </c>
       <c r="L234" t="n">
-        <v>0.0762686942321425</v>
+        <v>0.0763467499494172</v>
       </c>
       <c r="M234" t="n">
         <v>0</v>
@@ -24745,25 +24745,25 @@
         <v>0</v>
       </c>
       <c r="R234" t="n">
-        <v>-0.011075958682872</v>
+        <v>-0.0110872941581702</v>
       </c>
       <c r="S234" t="n">
-        <v>-0.0427124436743467</v>
+        <v>-0.0427434706441616</v>
       </c>
       <c r="T234" t="n">
-        <v>0.000197993569335178</v>
+        <v>0.000198196202017248</v>
       </c>
       <c r="U234" t="n">
-        <v>-0.00101567675445082</v>
+        <v>-0.00101647258062486</v>
       </c>
       <c r="V234" t="n">
         <v>0</v>
       </c>
       <c r="W234" t="n">
-        <v>-0.00133774936706897</v>
+        <v>-0.0013391184607375</v>
       </c>
       <c r="X234" t="n">
-        <v>-0.0000781239682923242</v>
+        <v>-0.0000789315743194783</v>
       </c>
       <c r="Y234" t="n">
         <v>0</v>
@@ -24778,19 +24778,19 @@
         <v>0</v>
       </c>
       <c r="AC234" t="n">
-        <v>5.67604888531145</v>
+        <v>5.68185792755991</v>
       </c>
       <c r="AD234" t="n">
-        <v>-0.0560219588776956</v>
+        <v>-0.0560670912159963</v>
       </c>
       <c r="AE234" t="n">
-        <v>5.62002692643375</v>
+        <v>5.62579083634391</v>
       </c>
       <c r="AF234" t="n">
-        <v>5.62002692643375</v>
+        <v>5.62579083634391</v>
       </c>
       <c r="AG234" t="n">
-        <v>5.67796436605856</v>
+        <v>5.68366977393735</v>
       </c>
     </row>
     <row r="235">
@@ -24798,7 +24798,7 @@
         <v>268</v>
       </c>
       <c r="B235" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C235" t="n">
         <v>0</v>
@@ -24822,13 +24822,13 @@
         <v>0</v>
       </c>
       <c r="J235" t="n">
-        <v>0.212184666833026</v>
+        <v>0.212401823118853</v>
       </c>
       <c r="K235" t="n">
         <v>0</v>
       </c>
       <c r="L235" t="n">
-        <v>0.0754831207954428</v>
+        <v>0.0755603725328056</v>
       </c>
       <c r="M235" t="n">
         <v>0</v>
@@ -24849,13 +24849,13 @@
         <v>0</v>
       </c>
       <c r="S235" t="n">
-        <v>-0.0319518157034457</v>
+        <v>-0.0321353475518663</v>
       </c>
       <c r="T235" t="n">
-        <v>0.000194276032745992</v>
+        <v>0.000194474860787273</v>
       </c>
       <c r="U235" t="n">
-        <v>-0.000599872205572972</v>
+        <v>-0.000600365375839933</v>
       </c>
       <c r="V235" t="n">
         <v>0</v>
@@ -24864,7 +24864,7 @@
         <v>0</v>
       </c>
       <c r="X235" t="n">
-        <v>0</v>
+        <v>-0.0000773494265437505</v>
       </c>
       <c r="Y235" t="n">
         <v>0</v>
@@ -24879,19 +24879,19 @@
         <v>0</v>
       </c>
       <c r="AC235" t="n">
-        <v>0.287667787628469</v>
+        <v>0.287962195651659</v>
       </c>
       <c r="AD235" t="n">
-        <v>-0.0323574118762727</v>
+        <v>-0.0326185874934627</v>
       </c>
       <c r="AE235" t="n">
-        <v>0.255310375752196</v>
+        <v>0.255343608158196</v>
       </c>
       <c r="AF235" t="n">
-        <v>0.255310375752196</v>
+        <v>0.255343608158196</v>
       </c>
       <c r="AG235" t="n">
-        <v>4.30446596924482</v>
+        <v>4.30882360138777</v>
       </c>
     </row>
     <row r="236">
@@ -24899,7 +24899,7 @@
         <v>269</v>
       </c>
       <c r="B236" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C236" t="n">
         <v>0</v>
@@ -24923,13 +24923,13 @@
         <v>0</v>
       </c>
       <c r="J236" t="n">
-        <v>0.212245223050373</v>
+        <v>0.212462441311288</v>
       </c>
       <c r="K236" t="n">
         <v>0</v>
       </c>
       <c r="L236" t="n">
-        <v>0.0744670831559213</v>
+        <v>0.0745432950492494</v>
       </c>
       <c r="M236" t="n">
         <v>0</v>
@@ -24950,13 +24950,13 @@
         <v>0</v>
       </c>
       <c r="S236" t="n">
-        <v>-0.0315659597119268</v>
+        <v>-0.0315982652817492</v>
       </c>
       <c r="T236" t="n">
-        <v>0.000190618496672512</v>
+        <v>0.00019081358147937</v>
       </c>
       <c r="U236" t="n">
-        <v>-0.000597465951939578</v>
+        <v>-0.000598077416891159</v>
       </c>
       <c r="V236" t="n">
         <v>0</v>
@@ -24980,19 +24980,19 @@
         <v>0</v>
       </c>
       <c r="AC236" t="n">
-        <v>0.286712306206294</v>
+        <v>0.287005736360537</v>
       </c>
       <c r="AD236" t="n">
-        <v>-0.0319728071671939</v>
+        <v>-0.032005529117161</v>
       </c>
       <c r="AE236" t="n">
-        <v>0.2547394990391</v>
+        <v>0.255000207243376</v>
       </c>
       <c r="AF236" t="n">
-        <v>0.2547394990391</v>
+        <v>0.255000207243376</v>
       </c>
       <c r="AG236" t="n">
-        <v>2.94271563072269</v>
+        <v>2.94567643963519</v>
       </c>
     </row>
     <row r="237">
@@ -25000,7 +25000,7 @@
         <v>270</v>
       </c>
       <c r="B237" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C237" t="n">
         <v>0</v>
@@ -25024,13 +25024,13 @@
         <v>0</v>
       </c>
       <c r="J237" t="n">
-        <v>0.212330161489519</v>
+        <v>0.212547466679033</v>
       </c>
       <c r="K237" t="n">
         <v>0</v>
       </c>
       <c r="L237" t="n">
-        <v>0.073087878252101</v>
+        <v>0.0731626786248947</v>
       </c>
       <c r="M237" t="n">
         <v>0</v>
@@ -25051,13 +25051,13 @@
         <v>0</v>
       </c>
       <c r="S237" t="n">
-        <v>-0.0328780460871357</v>
+        <v>-0.0329116944863349</v>
       </c>
       <c r="T237" t="n">
-        <v>0.000440076988060572</v>
+        <v>0.000440527376326754</v>
       </c>
       <c r="U237" t="n">
-        <v>-0.000597571135814069</v>
+        <v>-0.000598182708414049</v>
       </c>
       <c r="V237" t="n">
         <v>0</v>
@@ -25081,19 +25081,19 @@
         <v>0</v>
       </c>
       <c r="AC237" t="n">
-        <v>0.28541803974162</v>
+        <v>0.285710145303928</v>
       </c>
       <c r="AD237" t="n">
-        <v>-0.0330355402348892</v>
+        <v>-0.0330693498184222</v>
       </c>
       <c r="AE237" t="n">
-        <v>0.252382499506731</v>
+        <v>0.252640795485506</v>
       </c>
       <c r="AF237" t="n">
-        <v>0.252382499506731</v>
+        <v>0.252640795485506</v>
       </c>
       <c r="AG237" t="n">
-        <v>1.59561482518294</v>
+        <v>1.59719386180775</v>
       </c>
     </row>
     <row r="238">
@@ -25101,7 +25101,7 @@
         <v>271</v>
       </c>
       <c r="B238" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C238" t="n">
         <v>0</v>
@@ -25125,13 +25125,13 @@
         <v>0</v>
       </c>
       <c r="J238" t="n">
-        <v>0.212436676767511</v>
+        <v>0.212654090968023</v>
       </c>
       <c r="K238" t="n">
         <v>0</v>
       </c>
       <c r="L238" t="n">
-        <v>0.0713795266575163</v>
+        <v>0.0714525786509729</v>
       </c>
       <c r="M238" t="n">
         <v>0</v>
@@ -25152,13 +25152,13 @@
         <v>0</v>
       </c>
       <c r="S238" t="n">
-        <v>-0.0320051888249726</v>
+        <v>-0.0320379439153199</v>
       </c>
       <c r="T238" t="n">
         <v>0</v>
       </c>
       <c r="U238" t="n">
-        <v>-0.000498821898175628</v>
+        <v>-0.000499332407781784</v>
       </c>
       <c r="V238" t="n">
         <v>0</v>
@@ -25182,19 +25182,19 @@
         <v>0</v>
       </c>
       <c r="AC238" t="n">
-        <v>0.283816203425027</v>
+        <v>0.284106669618995</v>
       </c>
       <c r="AD238" t="n">
-        <v>-0.0325040107231482</v>
+        <v>-0.0325372763231017</v>
       </c>
       <c r="AE238" t="n">
-        <v>0.251312192701879</v>
+        <v>0.251569393295894</v>
       </c>
       <c r="AF238" t="n">
-        <v>0.251312192701879</v>
+        <v>0.251569393295894</v>
       </c>
       <c r="AG238" t="n">
-        <v>0.253436141749976</v>
+        <v>0.253638501045744</v>
       </c>
     </row>
     <row r="239">
@@ -25202,7 +25202,7 @@
         <v>272</v>
       </c>
       <c r="B239" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C239" t="n">
         <v>0</v>
@@ -25253,13 +25253,13 @@
         <v>0</v>
       </c>
       <c r="S239" t="n">
-        <v>-0.0101298328833171</v>
+        <v>-0.0101402000644985</v>
       </c>
       <c r="T239" t="n">
         <v>0</v>
       </c>
       <c r="U239" t="n">
-        <v>-0.000393850137066904</v>
+        <v>-0.000394253215358161</v>
       </c>
       <c r="V239" t="n">
         <v>0</v>
@@ -25286,16 +25286,16 @@
         <v>0</v>
       </c>
       <c r="AD239" t="n">
-        <v>-0.010523683020384</v>
+        <v>-0.0105344532798567</v>
       </c>
       <c r="AE239" t="n">
-        <v>-0.010523683020384</v>
+        <v>-0.0105344532798567</v>
       </c>
       <c r="AF239" t="n">
-        <v>-0.010523683020384</v>
+        <v>-0.0105344532798567</v>
       </c>
       <c r="AG239" t="n">
-        <v>0.186977627056831</v>
+        <v>0.187168985686231</v>
       </c>
     </row>
     <row r="240">
@@ -25303,7 +25303,7 @@
         <v>273</v>
       </c>
       <c r="B240" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C240" t="n">
         <v>0</v>
@@ -25354,13 +25354,13 @@
         <v>0</v>
       </c>
       <c r="S240" t="n">
-        <v>-0.0100390605961659</v>
+        <v>-0.010049334878209</v>
       </c>
       <c r="T240" t="n">
         <v>0</v>
       </c>
       <c r="U240" t="n">
-        <v>-0.000291753106598129</v>
+        <v>-0.000292051695661858</v>
       </c>
       <c r="V240" t="n">
         <v>0</v>
@@ -25387,16 +25387,16 @@
         <v>0</v>
       </c>
       <c r="AD240" t="n">
-        <v>-0.010330813702764</v>
+        <v>-0.0103413865738709</v>
       </c>
       <c r="AE240" t="n">
-        <v>-0.010330813702764</v>
+        <v>-0.0103413865738709</v>
       </c>
       <c r="AF240" t="n">
-        <v>-0.010330813702764</v>
+        <v>-0.0103413865738709</v>
       </c>
       <c r="AG240" t="n">
-        <v>0.120710048871365</v>
+        <v>0.120833587231919</v>
       </c>
     </row>
     <row r="241">
@@ -25404,7 +25404,7 @@
         <v>274</v>
       </c>
       <c r="B241" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C241" t="n">
         <v>0</v>
@@ -25455,13 +25455,13 @@
         <v>0</v>
       </c>
       <c r="S241" t="n">
-        <v>-0.0103973296646899</v>
+        <v>-0.0104079706102691</v>
       </c>
       <c r="T241" t="n">
         <v>0</v>
       </c>
       <c r="U241" t="n">
-        <v>-0.000192500948243721</v>
+        <v>-0.000192697959609164</v>
       </c>
       <c r="V241" t="n">
         <v>0</v>
@@ -25488,16 +25488,16 @@
         <v>0</v>
       </c>
       <c r="AD241" t="n">
-        <v>-0.0105898306129336</v>
+        <v>-0.0106006685698782</v>
       </c>
       <c r="AE241" t="n">
-        <v>-0.0105898306129336</v>
+        <v>-0.0106006685698782</v>
       </c>
       <c r="AF241" t="n">
-        <v>-0.0105898306129336</v>
+        <v>-0.0106006685698782</v>
       </c>
       <c r="AG241" t="n">
-        <v>0.0549669663414493</v>
+        <v>0.0550232212180733</v>
       </c>
     </row>
     <row r="242">
@@ -25505,7 +25505,7 @@
         <v>275</v>
       </c>
       <c r="B242" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C242" t="n">
         <v>0</v>
@@ -25556,13 +25556,13 @@
         <v>0</v>
       </c>
       <c r="S242" t="n">
-        <v>-0.0100787888891693</v>
+        <v>-0.0100891038303641</v>
       </c>
       <c r="T242" t="n">
         <v>0</v>
       </c>
       <c r="U242" t="n">
-        <v>-0.0000960396789392872</v>
+        <v>-0.0000961379688877636</v>
       </c>
       <c r="V242" t="n">
         <v>0</v>
@@ -25589,16 +25589,16 @@
         <v>0</v>
       </c>
       <c r="AD242" t="n">
-        <v>-0.0101748285681086</v>
+        <v>-0.0101852417992518</v>
       </c>
       <c r="AE242" t="n">
-        <v>-0.0101748285681086</v>
+        <v>-0.0101852417992518</v>
       </c>
       <c r="AF242" t="n">
-        <v>-0.0101748285681086</v>
+        <v>-0.0101852417992518</v>
       </c>
       <c r="AG242" t="n">
-        <v>-0.0104047889760476</v>
+        <v>-0.010415437555713</v>
       </c>
     </row>
     <row r="243">
@@ -25606,7 +25606,7 @@
         <v>276</v>
       </c>
       <c r="B243" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C243" t="n">
         <v>0</v>
@@ -25699,7 +25699,7 @@
         <v>0</v>
       </c>
       <c r="AG243" t="n">
-        <v>-0.00777386822095162</v>
+        <v>-0.00778182423574885</v>
       </c>
     </row>
     <row r="244">
@@ -25707,7 +25707,7 @@
         <v>277</v>
       </c>
       <c r="B244" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C244" t="n">
         <v>0</v>
@@ -25800,7 +25800,7 @@
         <v>0</v>
       </c>
       <c r="AG244" t="n">
-        <v>-0.00519116479526061</v>
+        <v>-0.00519647759228114</v>
       </c>
     </row>
     <row r="245">
@@ -25808,7 +25808,7 @@
         <v>278</v>
       </c>
       <c r="B245" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C245" t="n">
         <v>0</v>
@@ -25901,7 +25901,7 @@
         <v>0</v>
       </c>
       <c r="AG245" t="n">
-        <v>-0.00254370714202721</v>
+        <v>-0.00254631044981158</v>
       </c>
     </row>
     <row r="246">
@@ -25909,7 +25909,7 @@
         <v>279</v>
       </c>
       <c r="B246" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C246" t="n">
         <v>0</v>
@@ -26002,7 +26002,7 @@
         <v>0</v>
       </c>
       <c r="AG246" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="247">
@@ -26010,7 +26010,7 @@
         <v>280</v>
       </c>
       <c r="B247" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C247" t="n">
         <v>0</v>
@@ -26103,7 +26103,7 @@
         <v>0</v>
       </c>
       <c r="AG247" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="248">
@@ -26111,7 +26111,7 @@
         <v>281</v>
       </c>
       <c r="B248" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C248" t="n">
         <v>0</v>
@@ -26204,7 +26204,7 @@
         <v>0</v>
       </c>
       <c r="AG248" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="249">
@@ -26212,7 +26212,7 @@
         <v>282</v>
       </c>
       <c r="B249" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C249" t="n">
         <v>0</v>
@@ -26305,7 +26305,7 @@
         <v>0</v>
       </c>
       <c r="AG249" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="250">
@@ -26313,7 +26313,7 @@
         <v>283</v>
       </c>
       <c r="B250" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C250" t="n">
         <v>0</v>
@@ -26406,7 +26406,7 @@
         <v>0</v>
       </c>
       <c r="AG250" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="251">
@@ -26414,7 +26414,7 @@
         <v>284</v>
       </c>
       <c r="B251" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C251" t="n">
         <v>0</v>
@@ -26507,7 +26507,7 @@
         <v>0</v>
       </c>
       <c r="AG251" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="252">
@@ -26515,7 +26515,7 @@
         <v>285</v>
       </c>
       <c r="B252" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C252" t="n">
         <v>0</v>
@@ -26608,7 +26608,7 @@
         <v>0</v>
       </c>
       <c r="AG252" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="253">
@@ -26616,7 +26616,7 @@
         <v>286</v>
       </c>
       <c r="B253" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C253" t="n">
         <v>0</v>
@@ -26709,7 +26709,7 @@
         <v>0</v>
       </c>
       <c r="AG253" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="254">
@@ -26717,7 +26717,7 @@
         <v>287</v>
       </c>
       <c r="B254" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C254" t="n">
         <v>0</v>
@@ -26810,7 +26810,7 @@
         <v>0</v>
       </c>
       <c r="AG254" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="255">
@@ -26818,7 +26818,7 @@
         <v>288</v>
       </c>
       <c r="B255" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C255" t="n">
         <v>0</v>
@@ -26911,7 +26911,7 @@
         <v>0</v>
       </c>
       <c r="AG255" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="256">
@@ -26919,7 +26919,7 @@
         <v>289</v>
       </c>
       <c r="B256" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C256" t="n">
         <v>0</v>
@@ -27012,7 +27012,7 @@
         <v>0</v>
       </c>
       <c r="AG256" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="257">
@@ -27020,7 +27020,7 @@
         <v>290</v>
       </c>
       <c r="B257" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C257" t="n">
         <v>0</v>
@@ -27113,7 +27113,7 @@
         <v>0</v>
       </c>
       <c r="AG257" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="258">
@@ -27121,7 +27121,7 @@
         <v>291</v>
       </c>
       <c r="B258" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C258" t="n">
         <v>0</v>
@@ -27214,7 +27214,7 @@
         <v>0</v>
       </c>
       <c r="AG258" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="259">
@@ -27222,7 +27222,7 @@
         <v>292</v>
       </c>
       <c r="B259" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C259" t="n">
         <v>0</v>
@@ -27315,7 +27315,7 @@
         <v>0</v>
       </c>
       <c r="AG259" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
     <row r="260">
@@ -27323,7 +27323,7 @@
         <v>293</v>
       </c>
       <c r="B260" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C260" t="n">
         <v>0</v>
@@ -27416,7 +27416,7 @@
         <v>0</v>
       </c>
       <c r="AG260" t="n">
-        <v>-0.0000000000000000503069808033274</v>
+        <v>0.00000000000000137693675905659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>